<commit_message>
Complete reworking the parsing method, show feedback on page
</commit_message>
<xml_diff>
--- a/docs/sample-import-data.xlsx
+++ b/docs/sample-import-data.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="347">
   <si>
     <t>Nume</t>
   </si>
@@ -184,36 +184,6 @@
   </si>
   <si>
     <t>Nota</t>
-  </si>
-  <si>
-    <t>30.11.2010</t>
-  </si>
-  <si>
-    <t>Ana</t>
-  </si>
-  <si>
-    <t>01.05.2015</t>
-  </si>
-  <si>
-    <t>pv 123</t>
-  </si>
-  <si>
-    <t>01.05.2016</t>
-  </si>
-  <si>
-    <t>Bogdan</t>
-  </si>
-  <si>
-    <t>B-3-4</t>
-  </si>
-  <si>
-    <t>15.03.2017</t>
-  </si>
-  <si>
-    <t>Cristian</t>
-  </si>
-  <si>
-    <t>din ...</t>
   </si>
   <si>
     <t>a-2-3</t>
@@ -1674,7 +1644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
@@ -1702,7 +1672,7 @@
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="28" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1728,7 +1698,7 @@
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="30" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1744,17 +1714,17 @@
     </row>
     <row r="14" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="29" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="29" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="29" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>7</v>
@@ -1768,7 +1738,7 @@
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="30" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -1776,7 +1746,7 @@
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="31" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -1784,7 +1754,7 @@
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="29" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -1792,7 +1762,7 @@
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="29" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -1814,12 +1784,12 @@
     </row>
     <row r="26" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A26" s="29" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="29" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>11</v>
@@ -1836,17 +1806,17 @@
     </row>
     <row r="31" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A31" s="29" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A32" s="29" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="29" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>14</v>
@@ -1857,7 +1827,7 @@
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="31" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -1865,7 +1835,7 @@
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="29" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -1873,7 +1843,7 @@
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="29" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -1898,7 +1868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
@@ -1906,24 +1876,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="26" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B2" s="27">
         <v>10</v>
@@ -1932,15 +1902,15 @@
         <v>5</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="26" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B3" s="27">
         <v>3</v>
@@ -1950,7 +1920,7 @@
       </c>
       <c r="D3" s="27"/>
       <c r="E3" s="27" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2644,7 +2614,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2657,22 +2627,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="16" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2774,7 +2744,7 @@
         <v>39</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>41</v>
@@ -2787,33 +2757,33 @@
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="19" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="15" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="F9" s="10"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="19" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="15" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="F10" s="15" t="s">
         <v>7</v>
@@ -2821,440 +2791,440 @@
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="19" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="15" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="F11" s="15"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="19" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="19" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="D13" s="11">
         <v>1000000</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="F13" s="10"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="19" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="15" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="F14" s="10"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="19" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="15" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="F15" s="10"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="19" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="15" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="F16" s="10"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="19" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="15" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="F17" s="10"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="19" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="15" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="F18" s="10"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="19" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="15" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="F19" s="10"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="19" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="15" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="F20" s="10"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="17"/>
       <c r="B21" s="15" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
       <c r="E21" s="15" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="F21" s="10"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="19" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="15" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="F22" s="10"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="19" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="15" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="F23" s="10"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="19" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="15" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="F24" s="10"/>
     </row>
     <row r="25" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A25" s="19" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="D25" s="11"/>
       <c r="E25" s="15" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="F25" s="10"/>
     </row>
     <row r="26" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A26" s="19" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="15" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="F26" s="10"/>
     </row>
     <row r="27" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A27" s="19" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="15" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="F27" s="10"/>
     </row>
     <row r="28" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A28" s="19" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="15" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="F28" s="10"/>
     </row>
     <row r="29" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A29" s="19" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="15" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="F29" s="10"/>
     </row>
     <row r="30" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A30" s="19" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="D30" s="11"/>
       <c r="E30" s="15" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="F30" s="10"/>
     </row>
     <row r="31" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A31" s="19" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="D31" s="11"/>
       <c r="E31" s="15" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="F31" s="10"/>
     </row>
     <row r="32" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A32" s="19" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="D32" s="11">
         <v>4000000</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="F32" s="10"/>
     </row>
     <row r="33" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A33" s="19" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="C33" s="11">
         <v>1202</v>
       </c>
       <c r="D33" s="11"/>
       <c r="E33" s="15" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="F33" s="10"/>
     </row>
     <row r="34" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A34" s="19" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="D34" s="11"/>
       <c r="E34" s="15" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="F34" s="10"/>
     </row>
     <row r="35" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A35" s="19" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="D35" s="11"/>
       <c r="E35" s="10" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="F35" s="10"/>
     </row>
     <row r="36" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A36" s="19" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="D36" s="11"/>
       <c r="E36" s="15" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="F36" s="10"/>
     </row>
     <row r="37" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A37" s="19" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="D37" s="11"/>
       <c r="E37" s="15" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="F37" s="10"/>
     </row>
     <row r="38" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A38" s="17"/>
       <c r="B38" s="15" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
@@ -3264,7 +3234,7 @@
     <row r="39" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="17"/>
       <c r="B39" s="15" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
@@ -3273,298 +3243,298 @@
     </row>
     <row r="40" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A40" s="19" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="15" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="F40" s="10"/>
     </row>
     <row r="41" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A41" s="19" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="D41" s="11"/>
       <c r="E41" s="15" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="F41" s="10"/>
     </row>
     <row r="42" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A42" s="19" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="15" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="F42" s="10"/>
     </row>
     <row r="43" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A43" s="19" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="D43" s="11"/>
       <c r="E43" s="15" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="F43" s="10"/>
     </row>
     <row r="44" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A44" s="19" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="D44" s="11"/>
       <c r="E44" s="15" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="F44" s="10"/>
     </row>
     <row r="45" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A45" s="19" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="D45" s="11"/>
       <c r="E45" s="15" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="F45" s="10"/>
     </row>
     <row r="46" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A46" s="19" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="D46" s="11"/>
       <c r="E46" s="15" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="F46" s="10"/>
     </row>
     <row r="47" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A47" s="19" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="D47" s="11"/>
       <c r="E47" s="15" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="F47" s="10"/>
     </row>
     <row r="48" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A48" s="19" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="C48" s="11"/>
       <c r="E48" s="15" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="F48" s="10"/>
     </row>
     <row r="49" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="19" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A50" s="19" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="D50" s="11"/>
       <c r="E50" s="15" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="F50" s="10"/>
     </row>
     <row r="51" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="19" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="D51" s="11"/>
       <c r="E51" s="15" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="F51" s="10"/>
     </row>
     <row r="52" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="19" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="D52" s="11"/>
       <c r="E52" s="15" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="F52" s="10"/>
     </row>
     <row r="53" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="19" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="D53" s="11"/>
       <c r="E53" s="15" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="F53" s="10"/>
     </row>
     <row r="54" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="19" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="D54" s="11"/>
       <c r="E54" s="15" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="F54" s="10"/>
     </row>
     <row r="55" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="19" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="D55" s="11"/>
       <c r="E55" s="15" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="F55" s="10"/>
     </row>
     <row r="56" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="19" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="D56" s="11">
         <v>700000</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="F56" s="15" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A57" s="19" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="D57" s="11"/>
       <c r="E57" s="15" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="F57" s="10"/>
     </row>
     <row r="58" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="17"/>
       <c r="B58" s="15" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C58" s="11"/>
       <c r="D58" s="11"/>
@@ -3574,7 +3544,7 @@
     <row r="59" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A59" s="17"/>
       <c r="B59" s="15" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="C59" s="11"/>
       <c r="D59" s="11"/>
@@ -3583,136 +3553,136 @@
     </row>
     <row r="60" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="19" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="D60" s="11"/>
       <c r="E60" s="15" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="F60" s="10"/>
     </row>
     <row r="61" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="19" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="D61" s="11"/>
       <c r="E61" s="15" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="F61" s="10"/>
     </row>
     <row r="62" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A62" s="19" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="D62" s="11"/>
       <c r="E62" s="15" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="F62" s="10"/>
     </row>
     <row r="63" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A63" s="19" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="D63" s="11"/>
       <c r="E63" s="15" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="F63" s="10"/>
     </row>
     <row r="64" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A64" s="19" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="D64" s="11"/>
       <c r="E64" s="15" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="F64" s="10"/>
     </row>
     <row r="65" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A65" s="19" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="D65" s="11"/>
       <c r="E65" s="15" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="F65" s="10"/>
     </row>
     <row r="66" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A66" s="19" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="D66" s="11"/>
       <c r="E66" s="15" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="F66" s="10"/>
     </row>
     <row r="67" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A67" s="19" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="D67" s="11"/>
       <c r="E67" s="15" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="F67" s="10"/>
     </row>
     <row r="68" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A68" s="17"/>
       <c r="B68" s="15" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="C68" s="11"/>
       <c r="D68" s="11"/>
@@ -3721,130 +3691,130 @@
     </row>
     <row r="69" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A69" s="19" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="D69" s="11"/>
       <c r="E69" s="15" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="F69" s="10"/>
     </row>
     <row r="70" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="19" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="D70" s="11"/>
       <c r="E70" s="15" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="F70" s="10"/>
     </row>
     <row r="71" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" s="19" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="D71" s="11"/>
       <c r="E71" s="15" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="F71" s="10"/>
     </row>
     <row r="72" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" s="17"/>
       <c r="B72" s="15" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C72" s="11"/>
       <c r="D72" s="11"/>
       <c r="E72" s="15" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="F72" s="10"/>
     </row>
     <row r="73" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="17"/>
       <c r="B73" s="15" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="C73" s="11"/>
       <c r="D73" s="11"/>
       <c r="E73" s="15" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="F73" s="10"/>
     </row>
     <row r="74" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" s="17"/>
       <c r="B74" s="15" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="C74" s="11"/>
       <c r="D74" s="11"/>
       <c r="E74" s="15" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="F74" s="10"/>
     </row>
     <row r="75" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="19" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="B75" s="15" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="D75" s="11"/>
       <c r="F75" s="10"/>
     </row>
     <row r="76" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="19" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="B76" s="15" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="D76" s="11"/>
       <c r="E76" s="15" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="F76" s="10"/>
     </row>
     <row r="77" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A77" s="19" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="B77" s="15" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="D77" s="11"/>
       <c r="E77" s="15" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="F77" s="10"/>
     </row>
@@ -4070,7 +4040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
@@ -4085,7 +4055,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>0</v>
@@ -4097,7 +4067,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4112,7 +4082,7 @@
         <v>23</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4124,10 +4094,10 @@
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4140,13 +4110,13 @@
         <v>31</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4163,55 +4133,55 @@
       </c>
       <c r="C7" s="23"/>
       <c r="D7" s="23" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B8" s="24" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="23" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C10" s="23"/>
       <c r="D10" s="23" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B11" s="24"/>
       <c r="C11" s="23"/>
@@ -4219,7 +4189,7 @@
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B12" s="24"/>
       <c r="C12" s="23"/>
@@ -4227,82 +4197,82 @@
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="23" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C14" s="23"/>
       <c r="D14" s="23" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C15" s="23"/>
       <c r="D15" s="23" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C16" s="23"/>
       <c r="D16" s="23" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C17" s="23"/>
       <c r="D17" s="23" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B18" s="24"/>
       <c r="C18" s="23"/>
@@ -4310,7 +4280,7 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B19" s="24"/>
       <c r="C19" s="23"/>
@@ -4318,7 +4288,7 @@
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B20" s="24"/>
       <c r="C20" s="23"/>
@@ -4326,7 +4296,7 @@
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="B21" s="24"/>
       <c r="C21" s="23"/>
@@ -4334,7 +4304,7 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B22" s="24"/>
       <c r="C22" s="23"/>
@@ -4342,7 +4312,7 @@
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="23" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B23" s="24"/>
       <c r="C23" s="23"/>
@@ -4350,7 +4320,7 @@
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="23" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B24" s="24"/>
       <c r="C24" s="23"/>
@@ -4358,7 +4328,7 @@
     </row>
     <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="23" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B25" s="24"/>
       <c r="C25" s="23"/>
@@ -4366,7 +4336,7 @@
     </row>
     <row r="26" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="23" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B26" s="24"/>
       <c r="C26" s="23"/>
@@ -4374,7 +4344,7 @@
     </row>
     <row r="27" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="23" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B27" s="24"/>
       <c r="C27" s="23"/>
@@ -4382,7 +4352,7 @@
     </row>
     <row r="28" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="23" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B28" s="24"/>
       <c r="C28" s="23"/>
@@ -4390,7 +4360,7 @@
     </row>
     <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="23" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="B29" s="24"/>
       <c r="C29" s="23"/>
@@ -4398,7 +4368,7 @@
     </row>
     <row r="30" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="23" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B30" s="24"/>
       <c r="C30" s="23"/>
@@ -4406,7 +4376,7 @@
     </row>
     <row r="31" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="23" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B31" s="24"/>
       <c r="C31" s="23"/>
@@ -4414,7 +4384,7 @@
     </row>
     <row r="32" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="23" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B32" s="24"/>
       <c r="C32" s="23"/>
@@ -4422,7 +4392,7 @@
     </row>
     <row r="33" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="23" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B33" s="24"/>
       <c r="C33" s="23"/>
@@ -4430,7 +4400,7 @@
     </row>
     <row r="34" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="23" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B34" s="24"/>
       <c r="C34" s="23"/>
@@ -4438,7 +4408,7 @@
     </row>
     <row r="35" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="23" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B35" s="24"/>
       <c r="C35" s="23"/>
@@ -4446,7 +4416,7 @@
     </row>
     <row r="36" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="23" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B36" s="24"/>
       <c r="C36" s="23"/>
@@ -4454,7 +4424,7 @@
     </row>
     <row r="37" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="23" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B37" s="24"/>
       <c r="C37" s="23"/>
@@ -4462,7 +4432,7 @@
     </row>
     <row r="38" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="23" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="B38" s="24"/>
       <c r="C38" s="23"/>
@@ -4470,7 +4440,7 @@
     </row>
     <row r="39" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="23" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B39" s="24"/>
       <c r="C39" s="23"/>
@@ -4478,7 +4448,7 @@
     </row>
     <row r="40" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="23" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B40" s="24"/>
       <c r="C40" s="23"/>
@@ -4486,7 +4456,7 @@
     </row>
     <row r="41" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" s="23" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="B41" s="24"/>
       <c r="C41" s="23"/>
@@ -4494,7 +4464,7 @@
     </row>
     <row r="42" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" s="23" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B42" s="24"/>
       <c r="C42" s="23"/>
@@ -4502,7 +4472,7 @@
     </row>
     <row r="43" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="23" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B43" s="24"/>
       <c r="C43" s="23"/>
@@ -4510,7 +4480,7 @@
     </row>
     <row r="44" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="23" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B44" s="24"/>
       <c r="C44" s="23"/>
@@ -4518,7 +4488,7 @@
     </row>
     <row r="45" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" s="23" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B45" s="24"/>
       <c r="C45" s="23"/>
@@ -4526,7 +4496,7 @@
     </row>
     <row r="46" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="23" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B46" s="24"/>
       <c r="C46" s="23"/>
@@ -4534,7 +4504,7 @@
     </row>
     <row r="47" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="23" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B47" s="24"/>
       <c r="C47" s="23"/>
@@ -4542,7 +4512,7 @@
     </row>
     <row r="48" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="23" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B48" s="24"/>
       <c r="C48" s="23"/>
@@ -4550,7 +4520,7 @@
     </row>
     <row r="49" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" s="23" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B49" s="24"/>
       <c r="C49" s="23"/>
@@ -4558,7 +4528,7 @@
     </row>
     <row r="50" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" s="23" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B50" s="24"/>
       <c r="C50" s="23"/>
@@ -4566,7 +4536,7 @@
     </row>
     <row r="51" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" s="23" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B51" s="24"/>
       <c r="C51" s="23"/>
@@ -4574,7 +4544,7 @@
     </row>
     <row r="52" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" s="23" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B52" s="24"/>
       <c r="C52" s="23"/>
@@ -4582,7 +4552,7 @@
     </row>
     <row r="53" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="23" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B53" s="24"/>
       <c r="C53" s="23"/>
@@ -4590,7 +4560,7 @@
     </row>
     <row r="54" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" s="23" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B54" s="24"/>
       <c r="C54" s="23"/>
@@ -4598,7 +4568,7 @@
     </row>
     <row r="55" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" s="23" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B55" s="24"/>
       <c r="C55" s="23"/>
@@ -4606,7 +4576,7 @@
     </row>
     <row r="56" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" s="23" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B56" s="24"/>
       <c r="C56" s="23"/>
@@ -4614,7 +4584,7 @@
     </row>
     <row r="57" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="23" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B57" s="24"/>
       <c r="C57" s="23"/>
@@ -4622,7 +4592,7 @@
     </row>
     <row r="58" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" s="23" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B58" s="24"/>
       <c r="C58" s="23"/>
@@ -4630,7 +4600,7 @@
     </row>
     <row r="59" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" s="23" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B59" s="24"/>
       <c r="C59" s="23"/>
@@ -4638,7 +4608,7 @@
     </row>
     <row r="60" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A60" s="23" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B60" s="24"/>
       <c r="C60" s="23"/>
@@ -4646,7 +4616,7 @@
     </row>
     <row r="61" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A61" s="23" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B61" s="24"/>
       <c r="C61" s="23"/>
@@ -4654,7 +4624,7 @@
     </row>
     <row r="62" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A62" s="23" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="B62" s="24"/>
       <c r="C62" s="23"/>
@@ -4662,7 +4632,7 @@
     </row>
     <row r="63" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A63" s="23" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B63" s="24"/>
       <c r="C63" s="23"/>
@@ -4670,7 +4640,7 @@
     </row>
     <row r="64" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B64" s="24"/>
       <c r="C64" s="23"/>
@@ -4678,7 +4648,7 @@
     </row>
     <row r="65" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A65" s="23" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B65" s="24"/>
       <c r="C65" s="23"/>
@@ -4686,7 +4656,7 @@
     </row>
     <row r="66" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A66" s="23" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B66" s="24"/>
       <c r="C66" s="23"/>
@@ -4694,7 +4664,7 @@
     </row>
     <row r="67" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A67" s="23" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="B67" s="24"/>
       <c r="C67" s="23"/>
@@ -4702,7 +4672,7 @@
     </row>
     <row r="68" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A68" s="23" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B68" s="24"/>
       <c r="C68" s="23"/>
@@ -4710,7 +4680,7 @@
     </row>
     <row r="69" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A69" s="23" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="B69" s="24"/>
       <c r="C69" s="23"/>
@@ -4718,7 +4688,7 @@
     </row>
     <row r="70" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A70" s="23" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="B70" s="24"/>
       <c r="C70" s="23"/>
@@ -4726,7 +4696,7 @@
     </row>
     <row r="71" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A71" s="23" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="B71" s="24"/>
       <c r="C71" s="23"/>
@@ -4734,7 +4704,7 @@
     </row>
     <row r="72" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A72" s="23" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B72" s="24"/>
       <c r="C72" s="23"/>
@@ -4742,7 +4712,7 @@
     </row>
     <row r="73" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A73" s="23" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="B73" s="24"/>
       <c r="C73" s="23"/>
@@ -4750,7 +4720,7 @@
     </row>
     <row r="74" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A74" s="23" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="B74" s="24"/>
       <c r="C74" s="23"/>
@@ -4758,7 +4728,7 @@
     </row>
     <row r="75" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A75" s="23" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="B75" s="24"/>
       <c r="C75" s="23"/>
@@ -4766,7 +4736,7 @@
     </row>
     <row r="76" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A76" s="23" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="B76" s="24"/>
       <c r="C76" s="23"/>
@@ -4774,7 +4744,7 @@
     </row>
     <row r="77" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A77" s="23" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B77" s="24"/>
       <c r="C77" s="23"/>
@@ -4905,7 +4875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
@@ -4993,13 +4963,13 @@
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="15" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="10"/>
       <c r="B8" s="15" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="10"/>
@@ -5010,7 +4980,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="10"/>
@@ -5021,7 +4991,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="10"/>
@@ -5030,7 +5000,7 @@
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="10"/>
       <c r="B11" s="15" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="10"/>
@@ -5039,7 +5009,7 @@
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="10"/>
       <c r="B12" s="15" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="10"/>
@@ -5048,7 +5018,7 @@
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="10"/>
       <c r="B13" s="15" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="10"/>
@@ -5059,7 +5029,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="10"/>
@@ -5070,7 +5040,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="10"/>
@@ -5081,14 +5051,14 @@
         <v>11</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="15" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5096,14 +5066,14 @@
         <v>11</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="15" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5111,7 +5081,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="10"/>
@@ -5120,7 +5090,7 @@
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="10"/>
       <c r="B19" s="15" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="10"/>
@@ -5129,7 +5099,7 @@
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="10"/>
       <c r="B20" s="15" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="10"/>
@@ -5138,7 +5108,7 @@
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="10"/>
       <c r="B21" s="15" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="10"/>
@@ -5149,7 +5119,7 @@
         <v>12</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="10"/>
@@ -5160,7 +5130,7 @@
         <v>12</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="10"/>
@@ -5169,7 +5139,7 @@
     <row r="24" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A24" s="10"/>
       <c r="B24" s="15" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="10"/>
@@ -5180,7 +5150,7 @@
         <v>12</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="10"/>
@@ -5191,7 +5161,7 @@
         <v>12</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="10"/>
@@ -5202,7 +5172,7 @@
         <v>12</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="10"/>
@@ -5213,7 +5183,7 @@
         <v>12</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="10"/>
@@ -5224,7 +5194,7 @@
         <v>12</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="10"/>
@@ -5235,7 +5205,7 @@
         <v>12</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="10"/>
@@ -5246,7 +5216,7 @@
         <v>12</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="10"/>
@@ -5257,7 +5227,7 @@
         <v>11</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="10"/>
@@ -5268,20 +5238,20 @@
         <v>11</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="15" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A34" s="10"/>
       <c r="B34" s="15" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="10"/>
@@ -5290,7 +5260,7 @@
     <row r="35" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A35" s="10"/>
       <c r="B35" s="15" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="10"/>
@@ -5301,7 +5271,7 @@
         <v>12</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C36" s="11"/>
       <c r="D36" s="10"/>
@@ -5312,7 +5282,7 @@
         <v>12</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C37" s="11"/>
       <c r="D37" s="10"/>
@@ -5323,7 +5293,7 @@
         <v>12</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="10"/>
@@ -5334,7 +5304,7 @@
         <v>12</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="10"/>
@@ -5345,7 +5315,7 @@
         <v>12</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="10"/>
@@ -5356,7 +5326,7 @@
         <v>12</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C41" s="11"/>
       <c r="D41" s="10"/>
@@ -5367,7 +5337,7 @@
         <v>12</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="10"/>
@@ -5378,7 +5348,7 @@
         <v>12</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C43" s="11"/>
       <c r="D43" s="10"/>
@@ -5389,7 +5359,7 @@
         <v>11</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C44" s="11"/>
       <c r="D44" s="10"/>
@@ -5400,7 +5370,7 @@
         <v>11</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="10"/>
@@ -5409,7 +5379,7 @@
     <row r="46" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A46" s="10"/>
       <c r="B46" s="15" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C46" s="11"/>
       <c r="D46" s="10"/>
@@ -5418,7 +5388,7 @@
     <row r="47" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A47" s="10"/>
       <c r="B47" s="15" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C47" s="11"/>
       <c r="D47" s="10"/>
@@ -5427,7 +5397,7 @@
     <row r="48" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A48" s="10"/>
       <c r="B48" s="15" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="C48" s="11"/>
       <c r="D48" s="10"/>
@@ -5436,7 +5406,7 @@
     <row r="49" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="10"/>
       <c r="B49" s="15" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="C49" s="11"/>
       <c r="D49" s="10"/>
@@ -5445,7 +5415,7 @@
     <row r="50" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A50" s="10"/>
       <c r="B50" s="15" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C50" s="11"/>
       <c r="D50" s="10"/>
@@ -5456,7 +5426,7 @@
         <v>11</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C51" s="11"/>
       <c r="D51" s="10"/>
@@ -5467,7 +5437,7 @@
         <v>11</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C52" s="11"/>
       <c r="D52" s="10"/>
@@ -5478,7 +5448,7 @@
         <v>11</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C53" s="11"/>
       <c r="D53" s="10"/>
@@ -5489,7 +5459,7 @@
         <v>11</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C54" s="11"/>
       <c r="D54" s="10"/>
@@ -5500,7 +5470,7 @@
         <v>12</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C55" s="11"/>
       <c r="D55" s="10"/>
@@ -5509,7 +5479,7 @@
     <row r="56" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="15"/>
       <c r="B56" s="15" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C56" s="11"/>
       <c r="D56" s="10"/>
@@ -5520,7 +5490,7 @@
         <v>11</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C57" s="11"/>
       <c r="D57" s="10"/>
@@ -5531,7 +5501,7 @@
         <v>12</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C58" s="11"/>
       <c r="D58" s="10"/>
@@ -5542,7 +5512,7 @@
         <v>12</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="C59" s="11"/>
       <c r="D59" s="10"/>
@@ -5553,7 +5523,7 @@
         <v>11</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C60" s="11"/>
       <c r="D60" s="10"/>
@@ -5564,7 +5534,7 @@
         <v>11</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C61" s="11"/>
       <c r="D61" s="10"/>
@@ -5575,7 +5545,7 @@
         <v>11</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="C62" s="11"/>
       <c r="D62" s="10"/>
@@ -5586,7 +5556,7 @@
         <v>11</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="C63" s="11"/>
       <c r="D63" s="10"/>
@@ -5597,7 +5567,7 @@
         <v>12</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C64" s="11"/>
       <c r="D64" s="10"/>
@@ -5608,7 +5578,7 @@
         <v>12</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="C65" s="11"/>
       <c r="D65" s="10"/>
@@ -5619,7 +5589,7 @@
         <v>11</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C66" s="11"/>
       <c r="D66" s="10"/>
@@ -5630,7 +5600,7 @@
         <v>11</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="C67" s="11"/>
       <c r="D67" s="10"/>
@@ -5641,7 +5611,7 @@
         <v>12</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="C68" s="11"/>
       <c r="D68" s="10"/>
@@ -5652,7 +5622,7 @@
         <v>11</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C69" s="11"/>
       <c r="D69" s="10"/>
@@ -5663,7 +5633,7 @@
         <v>12</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C70" s="11"/>
       <c r="D70" s="10"/>
@@ -5674,7 +5644,7 @@
         <v>12</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C71" s="11"/>
       <c r="D71" s="10"/>
@@ -5685,7 +5655,7 @@
         <v>11</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C72" s="11"/>
       <c r="D72" s="10"/>
@@ -5694,7 +5664,7 @@
     <row r="73" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="10"/>
       <c r="B73" s="15" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="C73" s="11"/>
       <c r="D73" s="10"/>
@@ -5705,7 +5675,7 @@
         <v>12</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="C74" s="11"/>
       <c r="D74" s="10"/>
@@ -5714,7 +5684,7 @@
     <row r="75" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="10"/>
       <c r="B75" s="15" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="C75" s="11"/>
       <c r="D75" s="10"/>
@@ -5723,7 +5693,7 @@
     <row r="76" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="10"/>
       <c r="B76" s="15" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="C76" s="11"/>
       <c r="D76" s="10"/>
@@ -5732,7 +5702,7 @@
     <row r="77" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A77" s="10"/>
       <c r="B77" s="15" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C77" s="11"/>
       <c r="D77" s="10"/>
@@ -5897,11 +5867,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E97"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A2:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5928,92 +5898,70 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="27"/>
-    </row>
-    <row r="3" spans="1:5" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" s="27"/>
-    </row>
-    <row r="5" spans="1:5" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>59</v>
-      </c>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="10"/>
+      <c r="B3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="10"/>
       <c r="B6" s="11" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+      <c r="A7" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="11">
+        <v>2014</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>281</v>
+      </c>
       <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="10"/>
-      <c r="B8" s="11" t="s">
-        <v>31</v>
+      <c r="B8" s="15" t="s">
+        <v>74</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -6021,8 +5969,8 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10"/>
-      <c r="B9" s="11" t="s">
-        <v>31</v>
+      <c r="B9" s="15" t="s">
+        <v>76</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -6030,26 +5978,20 @@
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="10"/>
-      <c r="B10" s="11" t="s">
-        <v>37</v>
+      <c r="B10" s="15" t="s">
+        <v>80</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="15" t="s">
-        <v>14</v>
-      </c>
+      <c r="A11" s="10"/>
       <c r="B11" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="11">
-        <v>2014</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>291</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="10"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6064,25 +6006,31 @@
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="10"/>
       <c r="B13" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="10"/>
+      <c r="A14" s="15" t="s">
+        <v>14</v>
+      </c>
       <c r="B14" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
+        <v>82</v>
+      </c>
+      <c r="C14" s="10">
+        <v>2011</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>282</v>
+      </c>
       <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="10"/>
       <c r="B15" s="15" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -6091,7 +6039,7 @@
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="10"/>
       <c r="B16" s="15" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -6100,37 +6048,43 @@
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="10"/>
       <c r="B17" s="15" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
     </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="15" t="s">
+    <row r="18" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A18" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="C18" s="10">
-        <v>2011</v>
+      <c r="B18" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>287</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E18" s="10"/>
     </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="10"/>
+    <row r="19" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A19" s="15" t="s">
+        <v>14</v>
+      </c>
       <c r="B19" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
+        <v>86</v>
+      </c>
+      <c r="C19" s="10">
+        <v>2004</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>167</v>
+      </c>
       <c r="E19" s="10"/>
     </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A20" s="10"/>
       <c r="B20" s="15" t="s">
         <v>87</v>
@@ -6139,61 +6093,67 @@
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
     </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="10"/>
       <c r="B21" s="15" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
     </row>
     <row r="22" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>297</v>
+      <c r="B22" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="10">
+        <v>2004</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="E22" s="10"/>
     </row>
     <row r="23" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="10"/>
+      <c r="B23" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A24" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="C23" s="10">
-        <v>2004</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="E23" s="10"/>
-    </row>
-    <row r="24" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A24" s="10"/>
       <c r="B24" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
+        <v>90</v>
+      </c>
+      <c r="C24" s="10">
+        <v>2015</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>284</v>
+      </c>
       <c r="E24" s="10"/>
     </row>
     <row r="25" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A25" s="10"/>
+      <c r="A25" s="15" t="s">
+        <v>14</v>
+      </c>
       <c r="B25" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
+        <v>91</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>286</v>
+      </c>
       <c r="E25" s="10"/>
     </row>
     <row r="26" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -6201,20 +6161,20 @@
         <v>14</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C26" s="10">
         <v>2004</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>293</v>
+        <v>182</v>
       </c>
       <c r="E26" s="10"/>
     </row>
     <row r="27" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A27" s="10"/>
       <c r="B27" s="15" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -6225,13 +6185,13 @@
         <v>14</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="C28" s="10">
-        <v>2015</v>
+        <v>2012</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>294</v>
+        <v>186</v>
       </c>
       <c r="E28" s="10"/>
     </row>
@@ -6240,13 +6200,13 @@
         <v>14</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>295</v>
+        <v>94</v>
+      </c>
+      <c r="C29" s="10">
+        <v>2010</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="E29" s="10"/>
     </row>
@@ -6255,20 +6215,20 @@
         <v>14</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C30" s="10">
-        <v>2004</v>
+        <v>2010</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>192</v>
+        <v>290</v>
       </c>
       <c r="E30" s="10"/>
     </row>
     <row r="31" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A31" s="10"/>
       <c r="B31" s="15" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
@@ -6279,50 +6239,38 @@
         <v>14</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="C32" s="10">
-        <v>2012</v>
+        <v>2014</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>196</v>
+        <v>291</v>
       </c>
       <c r="E32" s="10"/>
     </row>
     <row r="33" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A33" s="15" t="s">
-        <v>14</v>
-      </c>
+      <c r="A33" s="10"/>
       <c r="B33" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C33" s="10">
-        <v>2010</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>299</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
       <c r="E33" s="10"/>
     </row>
     <row r="34" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A34" s="15" t="s">
-        <v>14</v>
-      </c>
+      <c r="A34" s="10"/>
       <c r="B34" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="C34" s="10">
-        <v>2010</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>300</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
       <c r="E34" s="10"/>
     </row>
     <row r="35" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A35" s="10"/>
       <c r="B35" s="15" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
@@ -6333,38 +6281,44 @@
         <v>14</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C36" s="10">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="E36" s="10"/>
     </row>
     <row r="37" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A37" s="10"/>
       <c r="B37" s="15" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
     </row>
     <row r="38" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A38" s="10"/>
+      <c r="A38" s="15" t="s">
+        <v>14</v>
+      </c>
       <c r="B38" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
+        <v>103</v>
+      </c>
+      <c r="C38" s="10">
+        <v>2007</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>293</v>
+      </c>
       <c r="E38" s="10"/>
     </row>
     <row r="39" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="10"/>
       <c r="B39" s="15" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
@@ -6375,20 +6329,20 @@
         <v>14</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C40" s="10">
-        <v>2012</v>
+        <v>2004</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="E40" s="10"/>
     </row>
     <row r="41" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A41" s="10"/>
       <c r="B41" s="15" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
@@ -6399,86 +6353,80 @@
         <v>14</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C42" s="10">
-        <v>2007</v>
+        <v>2012</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="E42" s="10"/>
     </row>
     <row r="43" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A43" s="10"/>
       <c r="B43" s="15" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
     </row>
     <row r="44" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A44" s="15" t="s">
-        <v>14</v>
-      </c>
+      <c r="A44" s="10"/>
       <c r="B44" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="C44" s="10">
-        <v>2004</v>
-      </c>
-      <c r="D44" s="15" t="s">
-        <v>304</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
       <c r="E44" s="10"/>
     </row>
     <row r="45" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A45" s="10"/>
       <c r="B45" s="15" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C45" s="10"/>
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
     </row>
     <row r="46" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A46" s="15" t="s">
-        <v>14</v>
-      </c>
+      <c r="A46" s="10"/>
       <c r="B46" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="C46" s="10">
-        <v>2012</v>
-      </c>
-      <c r="D46" s="15" t="s">
-        <v>305</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
       <c r="E46" s="10"/>
     </row>
     <row r="47" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A47" s="10"/>
       <c r="B47" s="15" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C47" s="10"/>
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
     </row>
     <row r="48" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A48" s="10"/>
+      <c r="A48" s="15" t="s">
+        <v>14</v>
+      </c>
       <c r="B48" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
+        <v>113</v>
+      </c>
+      <c r="C48" s="10">
+        <v>2004</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>296</v>
+      </c>
       <c r="E48" s="10"/>
     </row>
     <row r="49" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="10"/>
       <c r="B49" s="15" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C49" s="10"/>
       <c r="D49" s="10"/>
@@ -6487,7 +6435,7 @@
     <row r="50" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A50" s="10"/>
       <c r="B50" s="15" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
@@ -6496,82 +6444,82 @@
     <row r="51" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="10"/>
       <c r="B51" s="15" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
     </row>
     <row r="52" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A52" s="15" t="s">
+      <c r="A52" s="10"/>
+      <c r="B52" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+    </row>
+    <row r="53" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A53" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B52" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="C52" s="10">
-        <v>2004</v>
-      </c>
-      <c r="D52" s="15" t="s">
-        <v>306</v>
-      </c>
-      <c r="E52" s="10"/>
-    </row>
-    <row r="53" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A53" s="10"/>
       <c r="B53" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
+        <v>117</v>
+      </c>
+      <c r="C53" s="10">
+        <v>2014</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>237</v>
+      </c>
       <c r="E53" s="10"/>
     </row>
     <row r="54" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="10"/>
       <c r="B54" s="15" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C54" s="10"/>
       <c r="D54" s="10"/>
       <c r="E54" s="10"/>
     </row>
     <row r="55" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A55" s="10"/>
+      <c r="A55" s="15" t="s">
+        <v>14</v>
+      </c>
       <c r="B55" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
+        <v>119</v>
+      </c>
+      <c r="C55" s="10">
+        <v>2002</v>
+      </c>
+      <c r="D55" s="15" t="s">
+        <v>297</v>
+      </c>
       <c r="E55" s="10"/>
     </row>
     <row r="56" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="10"/>
       <c r="B56" s="15" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C56" s="10"/>
       <c r="D56" s="10"/>
       <c r="E56" s="10"/>
     </row>
     <row r="57" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A57" s="15" t="s">
-        <v>14</v>
-      </c>
+      <c r="A57" s="10"/>
       <c r="B57" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="C57" s="10">
-        <v>2014</v>
-      </c>
-      <c r="D57" s="15" t="s">
-        <v>247</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
       <c r="E57" s="10"/>
     </row>
     <row r="58" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="10"/>
       <c r="B58" s="15" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C58" s="10"/>
       <c r="D58" s="10"/>
@@ -6582,20 +6530,20 @@
         <v>14</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C59" s="10">
-        <v>2002</v>
+        <v>2010</v>
       </c>
       <c r="D59" s="15" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="E59" s="10"/>
     </row>
     <row r="60" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="10"/>
       <c r="B60" s="15" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C60" s="10"/>
       <c r="D60" s="10"/>
@@ -6604,19 +6552,25 @@
     <row r="61" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="10"/>
       <c r="B61" s="15" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C61" s="10"/>
       <c r="D61" s="10"/>
       <c r="E61" s="10"/>
     </row>
     <row r="62" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A62" s="10"/>
+      <c r="A62" s="15" t="s">
+        <v>14</v>
+      </c>
       <c r="B62" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
+        <v>126</v>
+      </c>
+      <c r="C62" s="10">
+        <v>2007</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>299</v>
+      </c>
       <c r="E62" s="10"/>
     </row>
     <row r="63" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -6624,47 +6578,53 @@
         <v>14</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C63" s="10">
-        <v>2010</v>
+        <v>2004</v>
       </c>
       <c r="D63" s="15" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="E63" s="10"/>
     </row>
     <row r="64" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A64" s="10"/>
+      <c r="A64" s="15" t="s">
+        <v>14</v>
+      </c>
       <c r="B64" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
+        <v>128</v>
+      </c>
+      <c r="C64" s="10">
+        <v>2008</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>301</v>
+      </c>
       <c r="E64" s="10"/>
     </row>
     <row r="65" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A65" s="10"/>
+      <c r="A65" s="15" t="s">
+        <v>14</v>
+      </c>
       <c r="B65" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="C65" s="10"/>
-      <c r="D65" s="10"/>
+        <v>129</v>
+      </c>
+      <c r="C65" s="10">
+        <v>2005</v>
+      </c>
+      <c r="D65" s="15" t="s">
+        <v>302</v>
+      </c>
       <c r="E65" s="10"/>
     </row>
     <row r="66" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A66" s="15" t="s">
-        <v>14</v>
-      </c>
+      <c r="A66" s="10"/>
       <c r="B66" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="C66" s="10">
-        <v>2007</v>
-      </c>
-      <c r="D66" s="15" t="s">
-        <v>309</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
       <c r="E66" s="10"/>
     </row>
     <row r="67" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -6672,29 +6632,23 @@
         <v>14</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C67" s="10">
-        <v>2004</v>
+        <v>2008</v>
       </c>
       <c r="D67" s="15" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="E67" s="10"/>
     </row>
     <row r="68" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A68" s="15" t="s">
-        <v>14</v>
-      </c>
+      <c r="A68" s="10"/>
       <c r="B68" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="C68" s="10">
-        <v>2008</v>
-      </c>
-      <c r="D68" s="15" t="s">
-        <v>311</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="C68" s="10"/>
+      <c r="D68" s="10"/>
       <c r="E68" s="10"/>
     </row>
     <row r="69" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -6702,23 +6656,29 @@
         <v>14</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C69" s="10">
-        <v>2005</v>
+        <v>2007</v>
       </c>
       <c r="D69" s="15" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="E69" s="10"/>
     </row>
     <row r="70" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A70" s="10"/>
+      <c r="A70" s="15" t="s">
+        <v>14</v>
+      </c>
       <c r="B70" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="C70" s="10"/>
-      <c r="D70" s="10"/>
+        <v>134</v>
+      </c>
+      <c r="C70" s="10">
+        <v>2012</v>
+      </c>
+      <c r="D70" s="15" t="s">
+        <v>305</v>
+      </c>
       <c r="E70" s="10"/>
     </row>
     <row r="71" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -6726,38 +6686,32 @@
         <v>14</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C71" s="10">
-        <v>2008</v>
+        <v>2004</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="E71" s="10"/>
     </row>
     <row r="72" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" s="10"/>
       <c r="B72" s="15" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C72" s="10"/>
       <c r="D72" s="10"/>
       <c r="E72" s="10"/>
     </row>
     <row r="73" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A73" s="15" t="s">
-        <v>14</v>
-      </c>
+      <c r="A73" s="10"/>
       <c r="B73" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="C73" s="10">
-        <v>2007</v>
-      </c>
-      <c r="D73" s="15" t="s">
-        <v>314</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
       <c r="E73" s="10"/>
     </row>
     <row r="74" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -6765,13 +6719,13 @@
         <v>14</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C74" s="10">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="D74" s="15" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="E74" s="10"/>
     </row>
@@ -6780,20 +6734,20 @@
         <v>14</v>
       </c>
       <c r="B75" s="15" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C75" s="10">
-        <v>2004</v>
+        <v>2010</v>
       </c>
       <c r="D75" s="15" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="E75" s="10"/>
     </row>
     <row r="76" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="10"/>
       <c r="B76" s="15" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C76" s="10"/>
       <c r="D76" s="10"/>
@@ -6801,48 +6755,28 @@
     </row>
     <row r="77" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A77" s="10"/>
-      <c r="B77" s="15" t="s">
-        <v>147</v>
-      </c>
+      <c r="B77" s="10"/>
       <c r="C77" s="10"/>
       <c r="D77" s="10"/>
       <c r="E77" s="10"/>
     </row>
     <row r="78" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A78" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B78" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="C78" s="10">
-        <v>2010</v>
-      </c>
-      <c r="D78" s="15" t="s">
-        <v>317</v>
-      </c>
+      <c r="A78" s="10"/>
+      <c r="B78" s="10"/>
+      <c r="C78" s="10"/>
+      <c r="D78" s="10"/>
       <c r="E78" s="10"/>
     </row>
     <row r="79" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A79" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B79" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="C79" s="10">
-        <v>2010</v>
-      </c>
-      <c r="D79" s="15" t="s">
-        <v>318</v>
-      </c>
+      <c r="A79" s="10"/>
+      <c r="B79" s="10"/>
+      <c r="C79" s="10"/>
+      <c r="D79" s="10"/>
       <c r="E79" s="10"/>
     </row>
     <row r="80" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A80" s="10"/>
-      <c r="B80" s="15" t="s">
-        <v>150</v>
-      </c>
+      <c r="B80" s="10"/>
       <c r="C80" s="10"/>
       <c r="D80" s="10"/>
       <c r="E80" s="10"/>
@@ -6937,34 +6871,6 @@
       <c r="C93" s="10"/>
       <c r="D93" s="10"/>
       <c r="E93" s="10"/>
-    </row>
-    <row r="94" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A94" s="10"/>
-      <c r="B94" s="10"/>
-      <c r="C94" s="10"/>
-      <c r="D94" s="10"/>
-      <c r="E94" s="10"/>
-    </row>
-    <row r="95" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A95" s="10"/>
-      <c r="B95" s="10"/>
-      <c r="C95" s="10"/>
-      <c r="D95" s="10"/>
-      <c r="E95" s="10"/>
-    </row>
-    <row r="96" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A96" s="10"/>
-      <c r="B96" s="10"/>
-      <c r="C96" s="10"/>
-      <c r="D96" s="10"/>
-      <c r="E96" s="10"/>
-    </row>
-    <row r="97" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A97" s="10"/>
-      <c r="B97" s="10"/>
-      <c r="C97" s="10"/>
-      <c r="D97" s="10"/>
-      <c r="E97" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6975,7 +6881,7 @@
           <x14:formula1>
             <xm:f>Info!$B$33:$C$33</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A97</xm:sqref>
+          <xm:sqref>A2:A93</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6987,7 +6893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -6999,19 +6905,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="34" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B1" s="34" t="s">
         <v>47</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7025,7 +6931,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="E2" s="33">
         <v>30</v>
@@ -7039,13 +6945,13 @@
         <v>25</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7057,7 +6963,7 @@
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="27" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="E4" s="27">
         <v>20</v>
@@ -7072,7 +6978,7 @@
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="27" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="E5" s="27"/>
     </row>
@@ -7750,8 +7656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" zoomScale="206" zoomScaleNormal="206" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7761,26 +7667,26 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="26" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="26" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Add parsing for deeds; improve parsing framework
</commit_message>
<xml_diff>
--- a/docs/sample-import-data.xlsx
+++ b/docs/sample-import-data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="68800" yWindow="7000" windowWidth="33600" windowHeight="21000" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="21140" windowHeight="28260" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="346">
   <si>
     <t>Nume</t>
   </si>
@@ -1024,9 +1024,6 @@
   </si>
   <si>
     <t>Act</t>
-  </si>
-  <si>
-    <t>Locuri Veci</t>
   </si>
   <si>
     <t>Loc Veci</t>
@@ -1672,7 +1669,7 @@
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="28" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1698,7 +1695,7 @@
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="30" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1714,17 +1711,17 @@
     </row>
     <row r="14" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="29" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="29" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="29" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>7</v>
@@ -1738,7 +1735,7 @@
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="30" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -1754,7 +1751,7 @@
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="29" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -1762,7 +1759,7 @@
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="29" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -1784,12 +1781,12 @@
     </row>
     <row r="26" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A26" s="29" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="29" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>11</v>
@@ -1806,17 +1803,17 @@
     </row>
     <row r="31" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A31" s="29" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A32" s="29" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="29" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>14</v>
@@ -1827,7 +1824,7 @@
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="31" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -1835,7 +1832,7 @@
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="29" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -1843,7 +1840,7 @@
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="29" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -2612,9 +2609,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2630,7 +2627,7 @@
         <v>329</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>330</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>53</v>
@@ -4055,7 +4052,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>0</v>
@@ -5869,9 +5866,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A2:XFD5"/>
+      <selection pane="bottomLeft" activeCell="A64" sqref="A64:XFD64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Add construction parsing and possibility to get with relational keys
</commit_message>
<xml_diff>
--- a/docs/sample-import-data.xlsx
+++ b/docs/sample-import-data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="22060" windowHeight="28280"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25940" windowHeight="28280" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Operatii" sheetId="5" r:id="rId1"/>
@@ -1208,8 +1208,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1308,11 +1314,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1614,7 +1626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
@@ -4068,11 +4080,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G100"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4083,7 +4095,7 @@
     <col min="4" max="16384" width="14.5" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4096,11 +4108,11 @@
       <c r="D1" s="15" t="s">
         <v>324</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="E1" s="15" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="16" t="s">
         <v>12</v>
       </c>
@@ -4111,11 +4123,11 @@
       <c r="D2" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
         <v>12</v>
       </c>
@@ -4126,16 +4138,16 @@
       <c r="D3" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="G4" s="4" t="s">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E4" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="17" t="s">
         <v>301</v>
       </c>
@@ -4145,16 +4157,16 @@
       <c r="D5" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="G6" s="4" t="s">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E6" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="16" t="s">
         <v>14</v>
       </c>
@@ -4165,11 +4177,11 @@
       <c r="D7" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="16" t="s">
         <v>14</v>
       </c>
@@ -4180,21 +4192,21 @@
       <c r="D8" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
         <v>309</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="G9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="16" t="s">
         <v>138</v>
       </c>
@@ -4205,27 +4217,27 @@
       <c r="D10" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="16"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
-      <c r="G11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="16"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="G12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="16" t="s">
         <v>310</v>
       </c>
@@ -4236,11 +4248,11 @@
       <c r="D13" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="16" t="s">
         <v>146</v>
       </c>
@@ -4251,11 +4263,11 @@
       <c r="D14" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="16" t="s">
         <v>146</v>
       </c>
@@ -4266,11 +4278,11 @@
       <c r="D15" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="16" t="s">
         <v>149</v>
       </c>
@@ -4281,11 +4293,11 @@
       <c r="D16" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="16" t="s">
         <v>149</v>
       </c>
@@ -4296,501 +4308,501 @@
       <c r="D17" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="16"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
-      <c r="G18" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="16"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
-      <c r="G19" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="16"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
-      <c r="G20" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="16"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
-      <c r="G21" s="4" t="s">
+      <c r="E21" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="16"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
-      <c r="G22" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="16"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
-      <c r="G23" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="16"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
-      <c r="G24" s="4" t="s">
+      <c r="E24" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A25" s="16"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="G25" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A26" s="16"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
-      <c r="G26" s="4" t="s">
+      <c r="E26" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A27" s="16"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
-      <c r="G27" s="4" t="s">
+      <c r="E27" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A28" s="16"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
-      <c r="G28" s="4" t="s">
+      <c r="E28" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A29" s="16"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
-      <c r="G29" s="4" t="s">
+      <c r="E29" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A30" s="16"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
-      <c r="G30" s="4" t="s">
+      <c r="E30" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A31" s="16"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
-      <c r="G31" s="4" t="s">
+      <c r="E31" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A32" s="16"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
-      <c r="G32" s="4" t="s">
+      <c r="E32" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A33" s="16"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
-      <c r="G33" s="4" t="s">
+      <c r="E33" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A34" s="16"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
-      <c r="G34" s="4" t="s">
+      <c r="E34" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A35" s="16"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
-      <c r="G35" s="4" t="s">
+      <c r="E35" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A36" s="16"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
-      <c r="G36" s="4" t="s">
+      <c r="E36" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A37" s="16"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
-      <c r="G37" s="4" t="s">
+      <c r="E37" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A38" s="16"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
-      <c r="G38" s="4" t="s">
+      <c r="E38" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A39" s="16"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
-      <c r="G39" s="4" t="s">
+      <c r="E39" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A40" s="16"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
-      <c r="G40" s="4" t="s">
+      <c r="E40" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A41" s="16"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
-      <c r="G41" s="4" t="s">
+      <c r="E41" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A42" s="16"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
-      <c r="G42" s="4" t="s">
+      <c r="E42" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A43" s="16"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
-      <c r="G43" s="4" t="s">
+      <c r="E43" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A44" s="16"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
-      <c r="G44" s="4" t="s">
+      <c r="E44" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A45" s="16"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
-      <c r="G45" s="4" t="s">
+      <c r="E45" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A46" s="16"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
-      <c r="G46" s="4" t="s">
+      <c r="E46" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A47" s="16"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
-      <c r="G47" s="4" t="s">
+      <c r="E47" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A48" s="16"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
-      <c r="G48" s="4" t="s">
+      <c r="E48" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A49" s="16"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
-      <c r="G49" s="4" t="s">
+      <c r="E49" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A50" s="16"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
-      <c r="G50" s="4" t="s">
+      <c r="E50" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A51" s="16"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
-      <c r="G51" s="4" t="s">
+      <c r="E51" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A52" s="16"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
-      <c r="G52" s="4" t="s">
+      <c r="E52" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A53" s="16"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
-      <c r="G53" s="4" t="s">
+      <c r="E53" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A54" s="16"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
-      <c r="G54" s="4" t="s">
+      <c r="E54" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A55" s="16"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
-      <c r="G55" s="4" t="s">
+      <c r="E55" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A56" s="16"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
-      <c r="G56" s="4" t="s">
+      <c r="E56" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A57" s="16"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
-      <c r="G57" s="4" t="s">
+      <c r="E57" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A58" s="16"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
-      <c r="G58" s="4" t="s">
+      <c r="E58" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A59" s="16"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
-      <c r="G59" s="4" t="s">
+      <c r="E59" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A60" s="16"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
-      <c r="G60" s="4" t="s">
+      <c r="E60" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A61" s="16"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
-      <c r="G61" s="4" t="s">
+      <c r="E61" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A62" s="16"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
-      <c r="G62" s="4" t="s">
+      <c r="E62" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A63" s="16"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
-      <c r="G63" s="4" t="s">
+      <c r="E63" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A64" s="16"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
-      <c r="G64" s="4" t="s">
+      <c r="E64" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A65" s="16"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
-      <c r="G65" s="4" t="s">
+      <c r="E65" s="4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A66" s="16"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
-      <c r="G66" s="4" t="s">
+      <c r="E66" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A67" s="16"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
-      <c r="G67" s="4" t="s">
+      <c r="E67" s="4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A68" s="16"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
-      <c r="G68" s="4" t="s">
+      <c r="E68" s="4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A69" s="16"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
-      <c r="G69" s="4" t="s">
+      <c r="E69" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A70" s="16"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
-      <c r="G70" s="4" t="s">
+      <c r="E70" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A71" s="16"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
-      <c r="G71" s="4" t="s">
+      <c r="E71" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A72" s="16"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
-      <c r="G72" s="4" t="s">
+      <c r="E72" s="4" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A73" s="16"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
-      <c r="G73" s="4" t="s">
+      <c r="E73" s="4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A74" s="16"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
-      <c r="G74" s="4" t="s">
+      <c r="E74" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A75" s="16"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
-      <c r="G75" s="4" t="s">
+      <c r="E75" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A76" s="16"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
-      <c r="G76" s="4" t="s">
+      <c r="E76" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A77" s="16"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
-      <c r="G77" s="4" t="s">
+      <c r="E77" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A78" s="16"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
     </row>
-    <row r="79" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A79" s="16"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
     </row>
-    <row r="80" spans="1:7" ht="16" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A80" s="16"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>

</xml_diff>

<commit_message>
Organize fields: display, filter, search
</commit_message>
<xml_diff>
--- a/docs/sample-import-data.xlsx
+++ b/docs/sample-import-data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25940" windowHeight="28280" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="26040" windowHeight="28280" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Operatii" sheetId="5" r:id="rId1"/>
@@ -162,15 +162,9 @@
     <t>An</t>
   </si>
   <si>
-    <t>Suma asteptata</t>
-  </si>
-  <si>
     <t>Chitante</t>
   </si>
   <si>
-    <t>Valori chitante</t>
-  </si>
-  <si>
     <t>55/2015</t>
   </si>
   <si>
@@ -1012,6 +1006,12 @@
   </si>
   <si>
     <t>Optiuni alegeri multiple (pt afisare dropdown)</t>
+  </si>
+  <si>
+    <t>Sume asteptate</t>
+  </si>
+  <si>
+    <t>Sume platite</t>
   </si>
 </sst>
 </file>
@@ -1713,14 +1713,14 @@
         <v>2014</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -1729,7 +1729,7 @@
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -1738,7 +1738,7 @@
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -1747,7 +1747,7 @@
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -1756,7 +1756,7 @@
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4"/>
       <c r="B12" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -1765,7 +1765,7 @@
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -1776,20 +1776,20 @@
         <v>9</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C14" s="4">
         <v>2011</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -1798,7 +1798,7 @@
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -1807,7 +1807,7 @@
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -1821,10 +1821,10 @@
         <v>40</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E18" s="4"/>
     </row>
@@ -1833,20 +1833,20 @@
         <v>9</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C19" s="4">
         <v>2004</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -1855,7 +1855,7 @@
     <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -1866,20 +1866,20 @@
         <v>9</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C22" s="4">
         <v>2004</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A23" s="4"/>
       <c r="B23" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -1890,13 +1890,13 @@
         <v>9</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C24" s="4">
         <v>2015</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E24" s="4"/>
     </row>
@@ -1905,13 +1905,13 @@
         <v>9</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E25" s="4"/>
     </row>
@@ -1920,20 +1920,20 @@
         <v>9</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C26" s="4">
         <v>2004</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A27" s="4"/>
       <c r="B27" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -1944,13 +1944,13 @@
         <v>9</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C28" s="4">
         <v>2012</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E28" s="4"/>
     </row>
@@ -1959,13 +1959,13 @@
         <v>9</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C29" s="4">
         <v>2010</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E29" s="4"/>
     </row>
@@ -1974,20 +1974,20 @@
         <v>9</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C30" s="4">
         <v>2010</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E30" s="4"/>
     </row>
     <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A31" s="4"/>
       <c r="B31" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -1998,20 +1998,20 @@
         <v>9</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C32" s="4">
         <v>2014</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E32" s="4"/>
     </row>
     <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -2020,7 +2020,7 @@
     <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A34" s="4"/>
       <c r="B34" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -2029,7 +2029,7 @@
     <row r="35" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A35" s="4"/>
       <c r="B35" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
@@ -2040,20 +2040,20 @@
         <v>9</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C36" s="4">
         <v>2012</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E36" s="4"/>
     </row>
     <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A37" s="4"/>
       <c r="B37" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
@@ -2064,20 +2064,20 @@
         <v>9</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C38" s="4">
         <v>2007</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E38" s="4"/>
     </row>
     <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A39" s="4"/>
       <c r="B39" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
@@ -2088,20 +2088,20 @@
         <v>9</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C40" s="4">
         <v>2004</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E40" s="4"/>
     </row>
     <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A41" s="4"/>
       <c r="B41" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
@@ -2112,20 +2112,20 @@
         <v>9</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C42" s="4">
         <v>2012</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E42" s="4"/>
     </row>
     <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A43" s="4"/>
       <c r="B43" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
@@ -2134,7 +2134,7 @@
     <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A44" s="4"/>
       <c r="B44" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
@@ -2143,7 +2143,7 @@
     <row r="45" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A45" s="4"/>
       <c r="B45" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
@@ -2152,7 +2152,7 @@
     <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A46" s="4"/>
       <c r="B46" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
@@ -2161,7 +2161,7 @@
     <row r="47" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A47" s="4"/>
       <c r="B47" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
@@ -2172,20 +2172,20 @@
         <v>9</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C48" s="4">
         <v>2004</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E48" s="4"/>
     </row>
     <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A49" s="4"/>
       <c r="B49" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
@@ -2194,7 +2194,7 @@
     <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A50" s="4"/>
       <c r="B50" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
@@ -2203,7 +2203,7 @@
     <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A51" s="4"/>
       <c r="B51" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
@@ -2212,7 +2212,7 @@
     <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A52" s="4"/>
       <c r="B52" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
@@ -2223,20 +2223,20 @@
         <v>9</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C53" s="4">
         <v>2014</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E53" s="4"/>
     </row>
     <row r="54" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A54" s="4"/>
       <c r="B54" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
@@ -2247,20 +2247,20 @@
         <v>9</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C55" s="4">
         <v>2002</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E55" s="4"/>
     </row>
     <row r="56" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A56" s="4"/>
       <c r="B56" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
@@ -2269,7 +2269,7 @@
     <row r="57" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A57" s="4"/>
       <c r="B57" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
@@ -2278,7 +2278,7 @@
     <row r="58" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A58" s="4"/>
       <c r="B58" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
@@ -2289,20 +2289,20 @@
         <v>9</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C59" s="4">
         <v>2010</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E59" s="4"/>
     </row>
     <row r="60" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A60" s="4"/>
       <c r="B60" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
@@ -2311,7 +2311,7 @@
     <row r="61" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A61" s="4"/>
       <c r="B61" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
@@ -2322,13 +2322,13 @@
         <v>9</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C62" s="4">
         <v>2007</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E62" s="4"/>
     </row>
@@ -2337,13 +2337,13 @@
         <v>9</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C63" s="4">
         <v>2004</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E63" s="4"/>
     </row>
@@ -2352,13 +2352,13 @@
         <v>9</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C64" s="4">
         <v>2008</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E64" s="4"/>
     </row>
@@ -2367,20 +2367,20 @@
         <v>9</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C65" s="4">
         <v>2005</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E65" s="4"/>
     </row>
     <row r="66" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A66" s="4"/>
       <c r="B66" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
@@ -2391,20 +2391,20 @@
         <v>9</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C67" s="4">
         <v>2008</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E67" s="4"/>
     </row>
     <row r="68" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A68" s="4"/>
       <c r="B68" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
@@ -2415,13 +2415,13 @@
         <v>9</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C69" s="4">
         <v>2007</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E69" s="4"/>
     </row>
@@ -2430,13 +2430,13 @@
         <v>9</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C70" s="4">
         <v>2012</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E70" s="4"/>
     </row>
@@ -2445,20 +2445,20 @@
         <v>9</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C71" s="4">
         <v>2004</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E71" s="4"/>
     </row>
     <row r="72" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A72" s="4"/>
       <c r="B72" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
@@ -2467,7 +2467,7 @@
     <row r="73" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A73" s="4"/>
       <c r="B73" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
@@ -2478,13 +2478,13 @@
         <v>9</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C74" s="4">
         <v>2010</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E74" s="4"/>
     </row>
@@ -2493,20 +2493,20 @@
         <v>9</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C75" s="4">
         <v>2010</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E75" s="4"/>
     </row>
     <row r="76" spans="1:5" ht="16" x14ac:dyDescent="0.15">
       <c r="A76" s="4"/>
       <c r="B76" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
@@ -2654,7 +2654,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2669,22 +2669,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2786,7 +2786,7 @@
         <v>29</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>31</v>
@@ -2799,33 +2799,33 @@
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>4</v>
@@ -2833,440 +2833,440 @@
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D13" s="4">
         <v>1000000</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="13"/>
       <c r="B21" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>161</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>163</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>161</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>163</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A25" s="13" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A26" s="13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A27" s="13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A28" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A29" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A30" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A31" s="13" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A32" s="13" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D32" s="4">
         <v>4000000</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A33" s="13" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C33" s="4">
         <v>1202</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A34" s="13" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F34" s="4"/>
     </row>
     <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A35" s="13" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F35" s="4"/>
     </row>
     <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A36" s="13" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F36" s="4"/>
     </row>
     <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A37" s="13" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F37" s="4"/>
     </row>
     <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A38" s="13"/>
       <c r="B38" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
@@ -3276,7 +3276,7 @@
     <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A39" s="13"/>
       <c r="B39" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
@@ -3285,298 +3285,298 @@
     </row>
     <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A40" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F40" s="4"/>
     </row>
     <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A41" s="13" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F41" s="4"/>
     </row>
     <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A42" s="13" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A43" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F43" s="4"/>
     </row>
     <row r="44" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A44" s="13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F44" s="4"/>
     </row>
     <row r="45" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A45" s="13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F45" s="4"/>
     </row>
     <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A46" s="13" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F46" s="4"/>
     </row>
     <row r="47" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A47" s="13" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F47" s="4"/>
     </row>
     <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A48" s="13" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C48" s="4"/>
       <c r="E48" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F48" s="4"/>
     </row>
     <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A49" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="E49" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="B49" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C49" s="4" t="s">
+      <c r="F49" s="4" t="s">
         <v>216</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A50" s="13" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F50" s="4"/>
     </row>
     <row r="51" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A51" s="13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F51" s="4"/>
     </row>
     <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A52" s="13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F52" s="4"/>
     </row>
     <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A53" s="13" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F53" s="4"/>
     </row>
     <row r="54" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A54" s="13" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D54" s="4"/>
       <c r="E54" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F54" s="4"/>
     </row>
     <row r="55" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A55" s="13" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F55" s="4"/>
     </row>
     <row r="56" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A56" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D56" s="4">
         <v>700000</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A57" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F57" s="4"/>
     </row>
     <row r="58" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A58" s="13"/>
       <c r="B58" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
@@ -3586,7 +3586,7 @@
     <row r="59" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A59" s="13"/>
       <c r="B59" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
@@ -3595,136 +3595,136 @@
     </row>
     <row r="60" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A60" s="13" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F60" s="4"/>
     </row>
     <row r="61" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A61" s="13" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F61" s="4"/>
     </row>
     <row r="62" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A62" s="13" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D62" s="4"/>
       <c r="E62" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F62" s="4"/>
     </row>
     <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A63" s="13" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F63" s="4"/>
     </row>
     <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A64" s="13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F64" s="4"/>
     </row>
     <row r="65" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A65" s="13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F65" s="4"/>
     </row>
     <row r="66" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A66" s="13" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F66" s="4"/>
     </row>
     <row r="67" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A67" s="13" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F67" s="4"/>
     </row>
     <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A68" s="13"/>
       <c r="B68" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
@@ -3733,130 +3733,130 @@
     </row>
     <row r="69" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A69" s="13" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F69" s="4"/>
     </row>
     <row r="70" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A70" s="13" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F70" s="4"/>
     </row>
     <row r="71" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A71" s="13" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F71" s="4"/>
     </row>
     <row r="72" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A72" s="13"/>
       <c r="B72" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
       <c r="E72" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F72" s="4"/>
     </row>
     <row r="73" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A73" s="13"/>
       <c r="B73" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
       <c r="E73" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F73" s="4"/>
     </row>
     <row r="74" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A74" s="13"/>
       <c r="B74" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
       <c r="E74" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F74" s="4"/>
     </row>
     <row r="75" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A75" s="13" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D75" s="4"/>
       <c r="F75" s="4"/>
     </row>
     <row r="76" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A76" s="13" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F76" s="4"/>
     </row>
     <row r="77" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A77" s="13" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F77" s="4"/>
     </row>
@@ -4082,9 +4082,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4106,10 +4106,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4121,7 +4121,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>17</v>
@@ -4133,10 +4133,10 @@
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>19</v>
@@ -4149,13 +4149,13 @@
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="17" t="s">
+        <v>299</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>301</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>303</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>21</v>
@@ -4172,10 +4172,10 @@
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>30</v>
@@ -4187,38 +4187,38 @@
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4226,7 +4226,7 @@
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4234,82 +4234,82 @@
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="16" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="16" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="16" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4325,7 +4325,7 @@
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4333,7 +4333,7 @@
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="E20" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4341,7 +4341,7 @@
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="E21" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4349,7 +4349,7 @@
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4357,7 +4357,7 @@
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="E23" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4365,7 +4365,7 @@
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="E24" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4373,7 +4373,7 @@
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="E25" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4381,7 +4381,7 @@
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="E26" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4389,7 +4389,7 @@
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="E27" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4397,7 +4397,7 @@
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="E28" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4405,7 +4405,7 @@
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="E29" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4413,7 +4413,7 @@
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="E30" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4421,7 +4421,7 @@
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4429,7 +4429,7 @@
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="E32" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4437,7 +4437,7 @@
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="E33" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4445,7 +4445,7 @@
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="E34" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4453,7 +4453,7 @@
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="E35" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4461,7 +4461,7 @@
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="E36" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4469,7 +4469,7 @@
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="E37" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4477,7 +4477,7 @@
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="E38" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4485,7 +4485,7 @@
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="E39" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4493,7 +4493,7 @@
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="E40" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4501,7 +4501,7 @@
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="E41" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4509,7 +4509,7 @@
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="E42" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4517,7 +4517,7 @@
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="E43" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4525,7 +4525,7 @@
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="E44" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4533,7 +4533,7 @@
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="E45" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4541,7 +4541,7 @@
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="E46" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4549,7 +4549,7 @@
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="E47" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4557,7 +4557,7 @@
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="E48" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4565,7 +4565,7 @@
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="E49" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4573,7 +4573,7 @@
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="E50" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4581,7 +4581,7 @@
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="E51" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4589,7 +4589,7 @@
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="E52" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4597,7 +4597,7 @@
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="E53" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4605,7 +4605,7 @@
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="E54" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4613,7 +4613,7 @@
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="E55" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4621,7 +4621,7 @@
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="E56" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4629,7 +4629,7 @@
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="E57" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4637,7 +4637,7 @@
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="E58" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4645,7 +4645,7 @@
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="E59" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4653,7 +4653,7 @@
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="E60" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4661,7 +4661,7 @@
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="E61" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4669,7 +4669,7 @@
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="E62" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4677,7 +4677,7 @@
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="E63" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4685,7 +4685,7 @@
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="E64" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4693,7 +4693,7 @@
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="E65" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4701,7 +4701,7 @@
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
       <c r="E66" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4709,7 +4709,7 @@
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="E67" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4717,7 +4717,7 @@
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="E68" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4725,7 +4725,7 @@
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="E69" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4733,7 +4733,7 @@
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
       <c r="E70" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4741,7 +4741,7 @@
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="E71" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4749,7 +4749,7 @@
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="E72" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4757,7 +4757,7 @@
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="E73" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4765,7 +4765,7 @@
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="E74" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4773,7 +4773,7 @@
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="E75" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4781,7 +4781,7 @@
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
       <c r="E76" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -4789,7 +4789,7 @@
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
       <c r="E77" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="16" x14ac:dyDescent="0.15">
@@ -5007,13 +5007,13 @@
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="8"/>
       <c r="B8" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -5024,7 +5024,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -5035,7 +5035,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -5044,7 +5044,7 @@
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="8"/>
       <c r="B11" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
@@ -5053,7 +5053,7 @@
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="8"/>
       <c r="B12" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -5062,7 +5062,7 @@
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="8"/>
       <c r="B13" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -5073,7 +5073,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -5084,7 +5084,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -5095,14 +5095,14 @@
         <v>7</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="9" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5110,14 +5110,14 @@
         <v>7</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="9" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5134,7 +5134,7 @@
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="8"/>
       <c r="B19" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -5143,7 +5143,7 @@
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="8"/>
       <c r="B20" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -5152,7 +5152,7 @@
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="8"/>
       <c r="B21" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -5163,7 +5163,7 @@
         <v>8</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -5174,7 +5174,7 @@
         <v>8</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -5183,7 +5183,7 @@
     <row r="24" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A24" s="8"/>
       <c r="B24" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -5194,7 +5194,7 @@
         <v>8</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
@@ -5205,7 +5205,7 @@
         <v>8</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
@@ -5216,7 +5216,7 @@
         <v>8</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
@@ -5227,7 +5227,7 @@
         <v>8</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -5238,7 +5238,7 @@
         <v>8</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
@@ -5249,7 +5249,7 @@
         <v>8</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -5260,7 +5260,7 @@
         <v>8</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
@@ -5271,7 +5271,7 @@
         <v>7</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
@@ -5282,20 +5282,20 @@
         <v>7</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D33" s="8"/>
       <c r="E33" s="9" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A34" s="8"/>
       <c r="B34" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
@@ -5304,7 +5304,7 @@
     <row r="35" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A35" s="8"/>
       <c r="B35" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
@@ -5315,7 +5315,7 @@
         <v>8</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
@@ -5326,7 +5326,7 @@
         <v>8</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
@@ -5337,7 +5337,7 @@
         <v>8</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
@@ -5348,7 +5348,7 @@
         <v>8</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
@@ -5359,7 +5359,7 @@
         <v>8</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
@@ -5370,7 +5370,7 @@
         <v>8</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
@@ -5381,7 +5381,7 @@
         <v>8</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
@@ -5392,7 +5392,7 @@
         <v>8</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
@@ -5403,7 +5403,7 @@
         <v>7</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
@@ -5414,7 +5414,7 @@
         <v>7</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
@@ -5423,7 +5423,7 @@
     <row r="46" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A46" s="8"/>
       <c r="B46" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
@@ -5432,7 +5432,7 @@
     <row r="47" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A47" s="8"/>
       <c r="B47" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
@@ -5441,7 +5441,7 @@
     <row r="48" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A48" s="8"/>
       <c r="B48" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
@@ -5450,7 +5450,7 @@
     <row r="49" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="8"/>
       <c r="B49" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
@@ -5459,7 +5459,7 @@
     <row r="50" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A50" s="8"/>
       <c r="B50" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
@@ -5470,7 +5470,7 @@
         <v>7</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
@@ -5481,7 +5481,7 @@
         <v>7</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
@@ -5492,7 +5492,7 @@
         <v>7</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
@@ -5503,7 +5503,7 @@
         <v>7</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
@@ -5514,7 +5514,7 @@
         <v>8</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
@@ -5523,7 +5523,7 @@
     <row r="56" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="9"/>
       <c r="B56" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
@@ -5534,7 +5534,7 @@
         <v>7</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
@@ -5545,7 +5545,7 @@
         <v>8</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
@@ -5556,7 +5556,7 @@
         <v>8</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
@@ -5567,7 +5567,7 @@
         <v>7</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
@@ -5578,7 +5578,7 @@
         <v>7</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
@@ -5589,7 +5589,7 @@
         <v>7</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
@@ -5600,7 +5600,7 @@
         <v>7</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
@@ -5611,7 +5611,7 @@
         <v>8</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
@@ -5622,7 +5622,7 @@
         <v>8</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
@@ -5633,7 +5633,7 @@
         <v>7</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
@@ -5644,7 +5644,7 @@
         <v>7</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
@@ -5655,7 +5655,7 @@
         <v>8</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C68" s="8"/>
       <c r="D68" s="8"/>
@@ -5666,7 +5666,7 @@
         <v>7</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C69" s="8"/>
       <c r="D69" s="8"/>
@@ -5677,7 +5677,7 @@
         <v>8</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
@@ -5688,7 +5688,7 @@
         <v>8</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
@@ -5699,7 +5699,7 @@
         <v>7</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C72" s="8"/>
       <c r="D72" s="8"/>
@@ -5708,7 +5708,7 @@
     <row r="73" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="8"/>
       <c r="B73" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
@@ -5719,7 +5719,7 @@
         <v>8</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
@@ -5728,7 +5728,7 @@
     <row r="75" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="8"/>
       <c r="B75" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="8"/>
@@ -5737,7 +5737,7 @@
     <row r="76" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="8"/>
       <c r="B76" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
@@ -5746,7 +5746,7 @@
     <row r="77" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A77" s="8"/>
       <c r="B77" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C77" s="8"/>
       <c r="D77" s="8"/>
@@ -5913,9 +5913,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5931,16 +5931,16 @@
         <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>44</v>
+        <v>325</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="20" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5954,7 +5954,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E2" s="19">
         <v>30</v>
@@ -5968,13 +5968,13 @@
         <v>15</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="20" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5986,7 +5986,7 @@
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E4" s="22">
         <v>20</v>
@@ -6001,7 +6001,7 @@
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E5" s="22"/>
     </row>
@@ -6681,7 +6681,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6696,23 +6696,23 @@
         <v>41</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="20" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="20" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7124,24 +7124,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B2" s="24">
         <v>10</v>
@@ -7150,15 +7150,15 @@
         <v>5</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B3" s="24">
         <v>3</v>
@@ -7168,7 +7168,7 @@
       </c>
       <c r="D3" s="24"/>
       <c r="E3" s="24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7875,7 +7875,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="20" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7883,12 +7883,12 @@
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="27" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="28" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B4" s="29" t="s">
         <v>4</v>
@@ -7902,7 +7902,7 @@
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="28" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B5" s="29" t="s">
         <v>7</v>
@@ -7914,7 +7914,7 @@
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="28" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B6" s="29" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Add parser for payments, refactor admin page
</commit_message>
<xml_diff>
--- a/docs/sample-import-data.xlsx
+++ b/docs/sample-import-data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28200" windowHeight="28280" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="47000" windowHeight="28800" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Operatii" sheetId="5" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="348">
   <si>
     <t>Nume</t>
   </si>
@@ -911,60 +911,12 @@
     <t>Adus oseminte din</t>
   </si>
   <si>
-    <t>5/2000</t>
-  </si>
-  <si>
-    <t>99, 00, 01</t>
-  </si>
-  <si>
-    <t>20, 30, 30</t>
-  </si>
-  <si>
-    <t>30, 30</t>
-  </si>
-  <si>
-    <t>100/2000</t>
-  </si>
-  <si>
-    <t>a11, a11</t>
-  </si>
-  <si>
-    <t>a55, a55, a55</t>
-  </si>
-  <si>
-    <t>coloanele an, loc, platit reprezinta o unitate</t>
-  </si>
-  <si>
-    <t>numarul de ani trebuie sa corespunda cu numarul de locui si cu numarul de sume platite</t>
-  </si>
-  <si>
-    <t>daca numarul de locuri nu corespunde cu numarul de ani (eg: 99, 00, 01 si a55) se va repeta acelasi loc repetat cati ani sunt</t>
-  </si>
-  <si>
     <t>Ani</t>
   </si>
   <si>
-    <t>99, 00, 99, 00</t>
-  </si>
-  <si>
-    <t>a57, a57, b22, b22</t>
-  </si>
-  <si>
-    <t>20, 30, 20, 30</t>
-  </si>
-  <si>
-    <t>15, 16</t>
-  </si>
-  <si>
     <t>a13</t>
   </si>
   <si>
-    <t>14,15,16</t>
-  </si>
-  <si>
-    <t>daca numarul de sume platite nu corespunde cu numarul de ani, se va repeta suma platita cati ani sunt</t>
-  </si>
-  <si>
     <t>Totolan Ion</t>
   </si>
   <si>
@@ -1059,6 +1011,72 @@
   </si>
   <si>
     <t>a-4a-9, a-4b-9</t>
+  </si>
+  <si>
+    <t>a13, a14</t>
+  </si>
+  <si>
+    <t>14,15</t>
+  </si>
+  <si>
+    <t>20, 30</t>
+  </si>
+  <si>
+    <t>~&gt; a13,a14 | 14,15 | 30,30 (repetata aceeasi suma)</t>
+  </si>
+  <si>
+    <t>~&gt; a13,a13 | 14,15 | 20,30 (repetat acelasi loc)</t>
+  </si>
+  <si>
+    <t>~&gt; a13,a13 | 14,15 | 30,30 (repetat si locul si suma)</t>
+  </si>
+  <si>
+    <t>~&gt; a13,a14 | 14,15 | 20,30 (locuri diferite, sume diferite)</t>
+  </si>
+  <si>
+    <t>a-1-3</t>
+  </si>
+  <si>
+    <t>14, 15, 16</t>
+  </si>
+  <si>
+    <t>2/2015</t>
+  </si>
+  <si>
+    <t>a-1-4, a-1-5</t>
+  </si>
+  <si>
+    <t>98, 99</t>
+  </si>
+  <si>
+    <t>3/2015</t>
+  </si>
+  <si>
+    <t>a-1-6</t>
+  </si>
+  <si>
+    <t>00, 01</t>
+  </si>
+  <si>
+    <t>20, 25</t>
+  </si>
+  <si>
+    <t>4/2015</t>
+  </si>
+  <si>
+    <t>a-1-1</t>
+  </si>
+  <si>
+    <t>5/2015</t>
+  </si>
+  <si>
+    <t>a-1-7, a-1-8</t>
+  </si>
+  <si>
+    <t>5, 6</t>
+  </si>
+  <si>
+    <t>20, 20</t>
   </si>
 </sst>
 </file>
@@ -1261,7 +1279,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1321,8 +1339,30 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1369,9 +1409,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1402,9 +1439,6 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1426,7 +1460,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="81">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1456,6 +1490,17 @@
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1485,6 +1530,17 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1813,7 +1869,7 @@
         <v>35</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>290</v>
@@ -1865,7 +1921,7 @@
         <v>2011</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -1881,7 +1937,7 @@
         <v>2011</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -1945,7 +2001,7 @@
         <v>2008</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -1961,7 +2017,7 @@
         <v>2011</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -2514,16 +2570,16 @@
       <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="27" t="s">
         <v>278</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="27" t="s">
         <v>277</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="27" t="s">
         <v>276</v>
       </c>
     </row>
@@ -2531,33 +2587,33 @@
       <c r="A2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="30" t="s">
-        <v>314</v>
-      </c>
-      <c r="C2" s="30" t="s">
+      <c r="B2" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="C2" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30" t="s">
+      <c r="D2" s="28"/>
+      <c r="E2" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="30"/>
+      <c r="F2" s="28"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30" t="s">
+      <c r="D3" s="28"/>
+      <c r="E3" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="28" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2565,65 +2621,65 @@
       <c r="A4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30" t="s">
+      <c r="D4" s="28"/>
+      <c r="E4" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="30"/>
+      <c r="F4" s="28"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="30" t="s">
-        <v>315</v>
-      </c>
-      <c r="C5" s="30" t="s">
+      <c r="B5" s="28" t="s">
+        <v>299</v>
+      </c>
+      <c r="C5" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30" t="s">
+      <c r="D5" s="28"/>
+      <c r="E5" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="28"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30" t="s">
+      <c r="D6" s="28"/>
+      <c r="E6" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="F6" s="30"/>
+      <c r="F6" s="28"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30" t="s">
+      <c r="D7" s="28"/>
+      <c r="E7" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="28" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2631,477 +2687,477 @@
       <c r="A8" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30" t="s">
+      <c r="D8" s="28"/>
+      <c r="E8" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="F8" s="30"/>
+      <c r="F8" s="28"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30" t="s">
+      <c r="D9" s="28"/>
+      <c r="E9" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="F9" s="30"/>
+      <c r="F9" s="28"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D10" s="28">
         <v>1000000</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="E10" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="F10" s="30"/>
+      <c r="F10" s="28"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="B11" s="30" t="s">
-        <v>318</v>
-      </c>
-      <c r="C11" s="30" t="s">
+      <c r="B11" s="28" t="s">
+        <v>302</v>
+      </c>
+      <c r="C11" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30" t="s">
+      <c r="D11" s="28"/>
+      <c r="E11" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="F11" s="30"/>
+      <c r="F11" s="28"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30" t="s">
+      <c r="D12" s="28"/>
+      <c r="E12" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="F12" s="30"/>
+      <c r="F12" s="28"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30" t="s">
+      <c r="D13" s="28"/>
+      <c r="E13" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="F13" s="30"/>
+      <c r="F13" s="28"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30" t="s">
+      <c r="D14" s="28"/>
+      <c r="E14" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="F14" s="30"/>
+      <c r="F14" s="28"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30" t="s">
+      <c r="D15" s="28"/>
+      <c r="E15" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="F15" s="30"/>
+      <c r="F15" s="28"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30" t="s">
+      <c r="D16" s="28"/>
+      <c r="E16" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="F16" s="30"/>
+      <c r="F16" s="28"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="12"/>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30" t="s">
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="F17" s="30"/>
+      <c r="F17" s="28"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="B18" s="30" t="s">
-        <v>316</v>
-      </c>
-      <c r="C18" s="30" t="s">
+      <c r="B18" s="28" t="s">
+        <v>300</v>
+      </c>
+      <c r="C18" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30" t="s">
-        <v>317</v>
-      </c>
-      <c r="F18" s="30"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28" t="s">
+        <v>301</v>
+      </c>
+      <c r="F18" s="28"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="30" t="s">
+      <c r="C19" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30" t="s">
+      <c r="D19" s="28"/>
+      <c r="E19" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="F19" s="30"/>
+      <c r="F19" s="28"/>
     </row>
     <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A20" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="30" t="s">
+      <c r="C20" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30" t="s">
+      <c r="D20" s="28"/>
+      <c r="E20" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="F20" s="30"/>
+      <c r="F20" s="28"/>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A21" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="B21" s="30" t="s">
-        <v>334</v>
-      </c>
-      <c r="C21" s="30" t="s">
+      <c r="B21" s="28" t="s">
+        <v>318</v>
+      </c>
+      <c r="C21" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30" t="s">
+      <c r="D21" s="28"/>
+      <c r="E21" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="F21" s="30"/>
+      <c r="F21" s="28"/>
     </row>
     <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A22" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="B22" s="30" t="s">
-        <v>319</v>
-      </c>
-      <c r="C22" s="30" t="s">
+      <c r="B22" s="28" t="s">
+        <v>303</v>
+      </c>
+      <c r="C22" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30" t="s">
+      <c r="D22" s="28"/>
+      <c r="E22" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="F22" s="30"/>
+      <c r="F22" s="28"/>
     </row>
     <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A23" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="C23" s="30" t="s">
+      <c r="C23" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30" t="s">
+      <c r="D23" s="28"/>
+      <c r="E23" s="28" t="s">
         <v>152</v>
       </c>
-      <c r="F23" s="30"/>
+      <c r="F23" s="28"/>
     </row>
     <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A24" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="28" t="s">
         <v>154</v>
       </c>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30" t="s">
+      <c r="D24" s="28"/>
+      <c r="E24" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="F24" s="30"/>
+      <c r="F24" s="28"/>
     </row>
     <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A25" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="30" t="s">
+      <c r="C25" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="D25" s="30">
+      <c r="D25" s="28">
         <v>4000000</v>
       </c>
-      <c r="E25" s="30" t="s">
-        <v>337</v>
-      </c>
-      <c r="F25" s="30"/>
+      <c r="E25" s="28" t="s">
+        <v>321</v>
+      </c>
+      <c r="F25" s="28"/>
     </row>
     <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A26" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="C26" s="30" t="s">
-        <v>333</v>
-      </c>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30" t="s">
+      <c r="C26" s="28" t="s">
+        <v>317</v>
+      </c>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28" t="s">
         <v>159</v>
       </c>
-      <c r="F26" s="30"/>
+      <c r="F26" s="28"/>
     </row>
     <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A27" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="B27" s="30" t="s">
-        <v>335</v>
-      </c>
-      <c r="C27" s="30" t="s">
+      <c r="B27" s="28" t="s">
+        <v>319</v>
+      </c>
+      <c r="C27" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30" t="s">
-        <v>336</v>
-      </c>
-      <c r="F27" s="30"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28" t="s">
+        <v>320</v>
+      </c>
+      <c r="F27" s="28"/>
     </row>
     <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A28" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="C28" s="30" t="s">
+      <c r="C28" s="28" t="s">
         <v>163</v>
       </c>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30" t="s">
+      <c r="D28" s="28"/>
+      <c r="E28" s="28" t="s">
         <v>164</v>
       </c>
-      <c r="F28" s="30"/>
+      <c r="F28" s="28"/>
     </row>
     <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A29" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="30" t="s">
+      <c r="C29" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30" t="s">
+      <c r="D29" s="28"/>
+      <c r="E29" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="F29" s="30"/>
+      <c r="F29" s="28"/>
     </row>
     <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A30" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="30" t="s">
+      <c r="C30" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30" t="s">
+      <c r="D30" s="28"/>
+      <c r="E30" s="28" t="s">
         <v>169</v>
       </c>
-      <c r="F30" s="30"/>
+      <c r="F30" s="28"/>
     </row>
     <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A31" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="28" t="s">
         <v>172</v>
       </c>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30" t="s">
+      <c r="D31" s="28"/>
+      <c r="E31" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="F31" s="30"/>
+      <c r="F31" s="28"/>
     </row>
     <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A32" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="30" t="s">
+      <c r="C32" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30" t="s">
+      <c r="D32" s="28"/>
+      <c r="E32" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="F32" s="30"/>
+      <c r="F32" s="28"/>
     </row>
     <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A33" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="C33" s="30" t="s">
+      <c r="C33" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30" t="s">
+      <c r="D33" s="28"/>
+      <c r="E33" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="F33" s="30"/>
+      <c r="F33" s="28"/>
     </row>
     <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A34" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="B34" s="30" t="s">
-        <v>320</v>
-      </c>
-      <c r="C34" s="30" t="s">
+      <c r="B34" s="28" t="s">
+        <v>304</v>
+      </c>
+      <c r="C34" s="28" t="s">
         <v>179</v>
       </c>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30" t="s">
-        <v>321</v>
-      </c>
-      <c r="F34" s="30"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28" t="s">
+        <v>305</v>
+      </c>
+      <c r="F34" s="28"/>
     </row>
     <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A35" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="B35" s="30" t="s">
-        <v>323</v>
-      </c>
-      <c r="C35" s="30" t="s">
+      <c r="B35" s="28" t="s">
+        <v>307</v>
+      </c>
+      <c r="C35" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30" t="s">
+      <c r="D35" s="28"/>
+      <c r="E35" s="28" t="s">
         <v>182</v>
       </c>
-      <c r="F35" s="30"/>
+      <c r="F35" s="28"/>
     </row>
     <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A36" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="B36" s="30" t="s">
+      <c r="B36" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="C36" s="30"/>
-      <c r="E36" s="30" t="s">
+      <c r="C36" s="28"/>
+      <c r="E36" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="F36" s="30"/>
+      <c r="F36" s="28"/>
     </row>
     <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A37" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="B37" s="30" t="s">
+      <c r="B37" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="30" t="s">
+      <c r="C37" s="28" t="s">
         <v>186</v>
       </c>
-      <c r="E37" s="30" t="s">
+      <c r="E37" s="28" t="s">
         <v>187</v>
       </c>
-      <c r="F37" s="30" t="s">
+      <c r="F37" s="28" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3109,83 +3165,83 @@
       <c r="A38" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="B38" s="30" t="s">
+      <c r="B38" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="30" t="s">
+      <c r="C38" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30" t="s">
+      <c r="D38" s="28"/>
+      <c r="E38" s="28" t="s">
         <v>190</v>
       </c>
-      <c r="F38" s="30"/>
+      <c r="F38" s="28"/>
     </row>
     <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A39" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="B39" s="30" t="s">
-        <v>324</v>
-      </c>
-      <c r="C39" s="30" t="s">
+      <c r="B39" s="28" t="s">
+        <v>308</v>
+      </c>
+      <c r="C39" s="28" t="s">
         <v>192</v>
       </c>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30" t="s">
+      <c r="D39" s="28"/>
+      <c r="E39" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="F39" s="30"/>
+      <c r="F39" s="28"/>
     </row>
     <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A40" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="B40" s="30" t="s">
-        <v>325</v>
-      </c>
-      <c r="C40" s="30" t="s">
+      <c r="B40" s="28" t="s">
+        <v>309</v>
+      </c>
+      <c r="C40" s="28" t="s">
         <v>195</v>
       </c>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30" t="s">
+      <c r="D40" s="28"/>
+      <c r="E40" s="28" t="s">
         <v>196</v>
       </c>
-      <c r="F40" s="30"/>
+      <c r="F40" s="28"/>
     </row>
     <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A41" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="B41" s="30" t="s">
+      <c r="B41" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="C41" s="30" t="s">
+      <c r="C41" s="28" t="s">
         <v>198</v>
       </c>
-      <c r="D41" s="30"/>
-      <c r="E41" s="30" t="s">
+      <c r="D41" s="28"/>
+      <c r="E41" s="28" t="s">
         <v>202</v>
       </c>
-      <c r="F41" s="30"/>
+      <c r="F41" s="28"/>
     </row>
     <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A42" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="B42" s="30" t="s">
+      <c r="B42" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="C42" s="30" t="s">
+      <c r="C42" s="28" t="s">
         <v>201</v>
       </c>
-      <c r="D42" s="30">
+      <c r="D42" s="28">
         <v>700000</v>
       </c>
-      <c r="E42" s="30" t="s">
+      <c r="E42" s="28" t="s">
         <v>199</v>
       </c>
-      <c r="F42" s="30" t="s">
+      <c r="F42" s="28" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3193,382 +3249,382 @@
       <c r="A43" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="B43" s="30" t="s">
+      <c r="B43" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="30" t="s">
+      <c r="C43" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="D43" s="30"/>
-      <c r="E43" s="30" t="s">
+      <c r="D43" s="28"/>
+      <c r="E43" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="F43" s="30"/>
+      <c r="F43" s="28"/>
     </row>
     <row r="44" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A44" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="B44" s="30" t="s">
-        <v>326</v>
-      </c>
-      <c r="C44" s="30" t="s">
+      <c r="B44" s="28" t="s">
+        <v>310</v>
+      </c>
+      <c r="C44" s="28" t="s">
         <v>207</v>
       </c>
-      <c r="D44" s="30"/>
-      <c r="E44" s="30" t="s">
+      <c r="D44" s="28"/>
+      <c r="E44" s="28" t="s">
         <v>208</v>
       </c>
-      <c r="F44" s="30"/>
+      <c r="F44" s="28"/>
     </row>
     <row r="45" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A45" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="B45" s="30" t="s">
+      <c r="B45" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="C45" s="30" t="s">
+      <c r="C45" s="28" t="s">
         <v>210</v>
       </c>
-      <c r="D45" s="30"/>
-      <c r="E45" s="30" t="s">
+      <c r="D45" s="28"/>
+      <c r="E45" s="28" t="s">
         <v>211</v>
       </c>
-      <c r="F45" s="30"/>
+      <c r="F45" s="28"/>
     </row>
     <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A46" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="B46" s="30" t="s">
+      <c r="B46" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="C46" s="30" t="s">
+      <c r="C46" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="D46" s="30"/>
-      <c r="E46" s="30" t="s">
+      <c r="D46" s="28"/>
+      <c r="E46" s="28" t="s">
         <v>212</v>
       </c>
-      <c r="F46" s="30"/>
+      <c r="F46" s="28"/>
     </row>
     <row r="47" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A47" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="B47" s="30" t="s">
-        <v>327</v>
-      </c>
-      <c r="C47" s="30" t="s">
+      <c r="B47" s="28" t="s">
+        <v>311</v>
+      </c>
+      <c r="C47" s="28" t="s">
         <v>216</v>
       </c>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30" t="s">
+      <c r="D47" s="28"/>
+      <c r="E47" s="28" t="s">
         <v>217</v>
       </c>
-      <c r="F47" s="30"/>
+      <c r="F47" s="28"/>
     </row>
     <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A48" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="B48" s="30" t="s">
-        <v>328</v>
-      </c>
-      <c r="C48" s="30" t="s">
+      <c r="B48" s="28" t="s">
+        <v>312</v>
+      </c>
+      <c r="C48" s="28" t="s">
         <v>219</v>
       </c>
-      <c r="D48" s="30"/>
-      <c r="E48" s="30" t="s">
+      <c r="D48" s="28"/>
+      <c r="E48" s="28" t="s">
         <v>220</v>
       </c>
-      <c r="F48" s="30"/>
+      <c r="F48" s="28"/>
     </row>
     <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A49" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="B49" s="30" t="s">
+      <c r="B49" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="C49" s="30" t="s">
+      <c r="C49" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30" t="s">
+      <c r="D49" s="28"/>
+      <c r="E49" s="28" t="s">
         <v>223</v>
       </c>
-      <c r="F49" s="30"/>
+      <c r="F49" s="28"/>
     </row>
     <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A50" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="B50" s="30" t="s">
-        <v>329</v>
-      </c>
-      <c r="C50" s="30" t="s">
+      <c r="B50" s="28" t="s">
+        <v>313</v>
+      </c>
+      <c r="C50" s="28" t="s">
         <v>225</v>
       </c>
-      <c r="D50" s="30"/>
-      <c r="E50" s="30" t="s">
+      <c r="D50" s="28"/>
+      <c r="E50" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="F50" s="30"/>
+      <c r="F50" s="28"/>
     </row>
     <row r="51" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A51" s="12"/>
-      <c r="B51" s="30" t="s">
-        <v>330</v>
-      </c>
-      <c r="C51" s="30"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="30" t="s">
+      <c r="B51" s="28" t="s">
+        <v>314</v>
+      </c>
+      <c r="C51" s="28"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="F51" s="30"/>
+      <c r="F51" s="28"/>
     </row>
     <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A52" s="12"/>
-      <c r="B52" s="30" t="s">
+      <c r="B52" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="C52" s="30"/>
-      <c r="D52" s="30"/>
-      <c r="E52" s="30" t="s">
+      <c r="C52" s="28"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="F52" s="30"/>
+      <c r="F52" s="28"/>
     </row>
     <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A53" s="12" t="s">
         <v>229</v>
       </c>
-      <c r="B53" s="30" t="s">
+      <c r="B53" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="C53" s="30" t="s">
+      <c r="C53" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="D53" s="30"/>
-      <c r="F53" s="30"/>
+      <c r="D53" s="28"/>
+      <c r="F53" s="28"/>
     </row>
     <row r="54" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A54" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="B54" s="30" t="s">
-        <v>331</v>
-      </c>
-      <c r="C54" s="30" t="s">
+      <c r="B54" s="28" t="s">
+        <v>315</v>
+      </c>
+      <c r="C54" s="28" t="s">
         <v>232</v>
       </c>
-      <c r="D54" s="30"/>
-      <c r="E54" s="30" t="s">
+      <c r="D54" s="28"/>
+      <c r="E54" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="F54" s="30"/>
+      <c r="F54" s="28"/>
     </row>
     <row r="55" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A55" s="12"/>
-      <c r="B55" s="30"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="30"/>
-      <c r="F55" s="30"/>
+      <c r="B55" s="28"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="28"/>
     </row>
     <row r="56" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A56" s="12"/>
-      <c r="B56" s="30"/>
-      <c r="C56" s="30"/>
-      <c r="D56" s="30"/>
-      <c r="E56" s="30"/>
-      <c r="F56" s="30"/>
+      <c r="B56" s="28"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="28"/>
+      <c r="F56" s="28"/>
     </row>
     <row r="57" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A57" s="12"/>
-      <c r="B57" s="30"/>
-      <c r="C57" s="30"/>
-      <c r="D57" s="30"/>
-      <c r="E57" s="30"/>
-      <c r="F57" s="30"/>
+      <c r="B57" s="28"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="28"/>
+      <c r="E57" s="28"/>
+      <c r="F57" s="28"/>
     </row>
     <row r="58" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A58" s="12"/>
-      <c r="B58" s="30"/>
-      <c r="C58" s="30"/>
-      <c r="D58" s="30"/>
-      <c r="E58" s="30"/>
-      <c r="F58" s="30"/>
+      <c r="B58" s="28"/>
+      <c r="C58" s="28"/>
+      <c r="D58" s="28"/>
+      <c r="E58" s="28"/>
+      <c r="F58" s="28"/>
     </row>
     <row r="59" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A59" s="12"/>
-      <c r="B59" s="30"/>
-      <c r="C59" s="30"/>
-      <c r="D59" s="30"/>
-      <c r="E59" s="30"/>
-      <c r="F59" s="30"/>
+      <c r="B59" s="28"/>
+      <c r="C59" s="28"/>
+      <c r="D59" s="28"/>
+      <c r="E59" s="28"/>
+      <c r="F59" s="28"/>
     </row>
     <row r="60" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A60" s="12"/>
-      <c r="B60" s="30"/>
-      <c r="C60" s="30"/>
-      <c r="D60" s="30"/>
-      <c r="E60" s="30"/>
-      <c r="F60" s="30"/>
+      <c r="B60" s="28"/>
+      <c r="C60" s="28"/>
+      <c r="D60" s="28"/>
+      <c r="E60" s="28"/>
+      <c r="F60" s="28"/>
     </row>
     <row r="61" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A61" s="12"/>
-      <c r="B61" s="30"/>
-      <c r="C61" s="30"/>
-      <c r="D61" s="30"/>
-      <c r="E61" s="30"/>
-      <c r="F61" s="30"/>
+      <c r="B61" s="28"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="28"/>
+      <c r="E61" s="28"/>
+      <c r="F61" s="28"/>
     </row>
     <row r="62" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A62" s="12"/>
-      <c r="B62" s="30"/>
-      <c r="C62" s="30"/>
-      <c r="D62" s="30"/>
-      <c r="E62" s="30"/>
-      <c r="F62" s="30"/>
+      <c r="B62" s="28"/>
+      <c r="C62" s="28"/>
+      <c r="D62" s="28"/>
+      <c r="E62" s="28"/>
+      <c r="F62" s="28"/>
     </row>
     <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A63" s="12"/>
-      <c r="B63" s="30"/>
-      <c r="C63" s="30"/>
-      <c r="D63" s="30"/>
-      <c r="E63" s="30"/>
-      <c r="F63" s="30"/>
+      <c r="B63" s="28"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="28"/>
+      <c r="E63" s="28"/>
+      <c r="F63" s="28"/>
     </row>
     <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A64" s="12"/>
-      <c r="B64" s="30"/>
-      <c r="C64" s="30"/>
-      <c r="D64" s="30"/>
-      <c r="E64" s="30"/>
-      <c r="F64" s="30"/>
+      <c r="B64" s="28"/>
+      <c r="C64" s="28"/>
+      <c r="D64" s="28"/>
+      <c r="E64" s="28"/>
+      <c r="F64" s="28"/>
     </row>
     <row r="65" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A65" s="12"/>
-      <c r="B65" s="30"/>
-      <c r="C65" s="30"/>
-      <c r="D65" s="30"/>
-      <c r="E65" s="30"/>
-      <c r="F65" s="30"/>
+      <c r="B65" s="28"/>
+      <c r="C65" s="28"/>
+      <c r="D65" s="28"/>
+      <c r="E65" s="28"/>
+      <c r="F65" s="28"/>
     </row>
     <row r="66" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A66" s="12"/>
-      <c r="B66" s="30"/>
-      <c r="C66" s="30"/>
-      <c r="D66" s="30"/>
-      <c r="E66" s="30"/>
-      <c r="F66" s="30"/>
+      <c r="B66" s="28"/>
+      <c r="C66" s="28"/>
+      <c r="D66" s="28"/>
+      <c r="E66" s="28"/>
+      <c r="F66" s="28"/>
     </row>
     <row r="67" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A67" s="12"/>
-      <c r="B67" s="30"/>
-      <c r="C67" s="30"/>
-      <c r="D67" s="30"/>
-      <c r="E67" s="30"/>
-      <c r="F67" s="30"/>
+      <c r="B67" s="28"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="28"/>
+      <c r="E67" s="28"/>
+      <c r="F67" s="28"/>
     </row>
     <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A68" s="12"/>
-      <c r="B68" s="30"/>
-      <c r="C68" s="30"/>
-      <c r="D68" s="30"/>
-      <c r="E68" s="30"/>
-      <c r="F68" s="30"/>
+      <c r="B68" s="28"/>
+      <c r="C68" s="28"/>
+      <c r="D68" s="28"/>
+      <c r="E68" s="28"/>
+      <c r="F68" s="28"/>
     </row>
     <row r="69" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A69" s="12"/>
-      <c r="B69" s="30"/>
-      <c r="C69" s="30"/>
-      <c r="D69" s="30"/>
-      <c r="E69" s="30"/>
-      <c r="F69" s="30"/>
+      <c r="B69" s="28"/>
+      <c r="C69" s="28"/>
+      <c r="D69" s="28"/>
+      <c r="E69" s="28"/>
+      <c r="F69" s="28"/>
     </row>
     <row r="70" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A70" s="12"/>
-      <c r="B70" s="30"/>
-      <c r="C70" s="30"/>
-      <c r="D70" s="30"/>
-      <c r="E70" s="30"/>
-      <c r="F70" s="30"/>
+      <c r="B70" s="28"/>
+      <c r="C70" s="28"/>
+      <c r="D70" s="28"/>
+      <c r="E70" s="28"/>
+      <c r="F70" s="28"/>
     </row>
     <row r="71" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A71" s="12"/>
-      <c r="B71" s="30"/>
-      <c r="C71" s="30"/>
-      <c r="D71" s="30"/>
-      <c r="E71" s="30"/>
-      <c r="F71" s="30"/>
+      <c r="B71" s="28"/>
+      <c r="C71" s="28"/>
+      <c r="D71" s="28"/>
+      <c r="E71" s="28"/>
+      <c r="F71" s="28"/>
     </row>
     <row r="72" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A72" s="12"/>
-      <c r="B72" s="30"/>
-      <c r="C72" s="30"/>
-      <c r="D72" s="30"/>
-      <c r="E72" s="30"/>
-      <c r="F72" s="30"/>
+      <c r="B72" s="28"/>
+      <c r="C72" s="28"/>
+      <c r="D72" s="28"/>
+      <c r="E72" s="28"/>
+      <c r="F72" s="28"/>
     </row>
     <row r="73" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A73" s="12"/>
-      <c r="B73" s="30"/>
-      <c r="C73" s="30"/>
-      <c r="D73" s="30"/>
-      <c r="E73" s="30"/>
-      <c r="F73" s="30"/>
+      <c r="B73" s="28"/>
+      <c r="C73" s="28"/>
+      <c r="D73" s="28"/>
+      <c r="E73" s="28"/>
+      <c r="F73" s="28"/>
     </row>
     <row r="74" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A74" s="12"/>
-      <c r="B74" s="30"/>
-      <c r="C74" s="30"/>
-      <c r="D74" s="30"/>
-      <c r="E74" s="30"/>
-      <c r="F74" s="30"/>
+      <c r="B74" s="28"/>
+      <c r="C74" s="28"/>
+      <c r="D74" s="28"/>
+      <c r="E74" s="28"/>
+      <c r="F74" s="28"/>
     </row>
     <row r="75" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A75" s="12"/>
-      <c r="B75" s="30"/>
-      <c r="C75" s="30"/>
-      <c r="D75" s="30"/>
-      <c r="E75" s="30"/>
-      <c r="F75" s="30"/>
+      <c r="B75" s="28"/>
+      <c r="C75" s="28"/>
+      <c r="D75" s="28"/>
+      <c r="E75" s="28"/>
+      <c r="F75" s="28"/>
     </row>
     <row r="76" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A76" s="12"/>
-      <c r="B76" s="30"/>
-      <c r="C76" s="30"/>
-      <c r="D76" s="30"/>
-      <c r="E76" s="30"/>
-      <c r="F76" s="30"/>
+      <c r="B76" s="28"/>
+      <c r="C76" s="28"/>
+      <c r="D76" s="28"/>
+      <c r="E76" s="28"/>
+      <c r="F76" s="28"/>
     </row>
     <row r="77" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A77" s="12"/>
-      <c r="B77" s="30"/>
-      <c r="C77" s="30"/>
-      <c r="D77" s="30"/>
-      <c r="E77" s="30"/>
-      <c r="F77" s="30"/>
+      <c r="B77" s="28"/>
+      <c r="C77" s="28"/>
+      <c r="D77" s="28"/>
+      <c r="E77" s="28"/>
+      <c r="F77" s="28"/>
     </row>
     <row r="78" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A78" s="12"/>
-      <c r="B78" s="30"/>
-      <c r="C78" s="30"/>
-      <c r="D78" s="30"/>
-      <c r="E78" s="30"/>
-      <c r="F78" s="30"/>
+      <c r="B78" s="28"/>
+      <c r="C78" s="28"/>
+      <c r="D78" s="28"/>
+      <c r="E78" s="28"/>
+      <c r="F78" s="28"/>
     </row>
     <row r="79" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A79" s="12"/>
-      <c r="B79" s="30"/>
-      <c r="C79" s="30"/>
-      <c r="D79" s="30"/>
-      <c r="E79" s="30"/>
-      <c r="F79" s="30"/>
+      <c r="B79" s="28"/>
+      <c r="C79" s="28"/>
+      <c r="D79" s="28"/>
+      <c r="E79" s="28"/>
+      <c r="F79" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4219,14 +4275,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A37" sqref="A37:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="25" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="24" customWidth="1"/>
     <col min="2" max="2" width="15.1640625" style="7" customWidth="1"/>
     <col min="3" max="3" width="17.1640625" style="7" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" style="7" customWidth="1"/>
@@ -4251,7 +4307,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -4262,7 +4318,7 @@
       <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -4277,7 +4333,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -4288,7 +4344,7 @@
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -4299,22 +4355,22 @@
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>318</v>
+        <v>302</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>338</v>
+        <v>322</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>234</v>
@@ -4325,7 +4381,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -4336,18 +4392,18 @@
       <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -4358,29 +4414,29 @@
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>334</v>
+        <v>318</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
     </row>
     <row r="12" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>319</v>
+        <v>303</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="8" t="s">
@@ -4391,7 +4447,7 @@
       <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -4402,7 +4458,7 @@
       <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="8" t="s">
@@ -4413,7 +4469,7 @@
       <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="8" t="s">
@@ -4428,7 +4484,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="8" t="s">
@@ -4439,7 +4495,7 @@
       <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="8" t="s">
@@ -4450,29 +4506,29 @@
       <c r="E18" s="8"/>
     </row>
     <row r="19" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>339</v>
+        <v>323</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="8" t="s">
@@ -4483,7 +4539,7 @@
       <c r="E21" s="8"/>
     </row>
     <row r="22" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="8" t="s">
@@ -4494,40 +4550,40 @@
       <c r="E22" s="8"/>
     </row>
     <row r="23" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>324</v>
+        <v>308</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
     </row>
     <row r="25" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>325</v>
+        <v>309</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B26" s="8" t="s">
@@ -4538,7 +4594,7 @@
       <c r="E26" s="8"/>
     </row>
     <row r="27" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B27" s="8" t="s">
@@ -4549,29 +4605,29 @@
       <c r="E27" s="8"/>
     </row>
     <row r="28" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
     </row>
     <row r="29" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>326</v>
+        <v>310</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
     </row>
     <row r="30" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="8" t="s">
@@ -4582,7 +4638,7 @@
       <c r="E30" s="8"/>
     </row>
     <row r="31" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B31" s="8" t="s">
@@ -4593,29 +4649,29 @@
       <c r="E31" s="8"/>
     </row>
     <row r="32" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A32" s="24" t="s">
+      <c r="A32" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
     </row>
     <row r="33" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
     </row>
     <row r="34" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A34" s="24" t="s">
+      <c r="A34" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B34" s="8" t="s">
@@ -4626,7 +4682,7 @@
       <c r="E34" s="8"/>
     </row>
     <row r="35" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A35" s="24" t="s">
+      <c r="A35" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B35" s="8" t="s">
@@ -4637,18 +4693,18 @@
       <c r="E35" s="8"/>
     </row>
     <row r="36" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A36" s="24" t="s">
+      <c r="A36" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
     </row>
     <row r="37" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A37" s="24" t="s">
+      <c r="A37" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B37" s="8" t="s">
@@ -4659,7 +4715,7 @@
       <c r="E37" s="8"/>
     </row>
     <row r="38" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A38" s="24" t="s">
+      <c r="A38" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B38" s="8" t="s">
@@ -4670,140 +4726,140 @@
       <c r="E38" s="8"/>
     </row>
     <row r="39" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A39" s="24"/>
+      <c r="A39" s="23"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
     </row>
     <row r="40" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A40" s="24"/>
+      <c r="A40" s="23"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
     </row>
     <row r="41" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A41" s="24"/>
+      <c r="A41" s="23"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A42" s="24"/>
+      <c r="A42" s="23"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
     </row>
     <row r="43" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A43" s="24"/>
+      <c r="A43" s="23"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
     </row>
     <row r="44" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A44" s="24"/>
+      <c r="A44" s="23"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
     </row>
     <row r="45" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A45" s="24"/>
+      <c r="A45" s="23"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
     </row>
     <row r="46" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A46" s="24"/>
+      <c r="A46" s="23"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
     </row>
     <row r="47" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A47" s="24"/>
+      <c r="A47" s="23"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
     </row>
     <row r="48" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A48" s="24"/>
+      <c r="A48" s="23"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
     </row>
     <row r="49" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A49" s="24"/>
+      <c r="A49" s="23"/>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
     </row>
     <row r="50" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A50" s="24"/>
+      <c r="A50" s="23"/>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
     </row>
     <row r="51" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A51" s="24"/>
+      <c r="A51" s="23"/>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
       <c r="E51" s="8"/>
     </row>
     <row r="52" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A52" s="24"/>
+      <c r="A52" s="23"/>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
       <c r="E52" s="8"/>
     </row>
     <row r="53" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A53" s="24"/>
+      <c r="A53" s="23"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
       <c r="E53" s="8"/>
     </row>
     <row r="54" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A54" s="24"/>
+      <c r="A54" s="23"/>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
       <c r="E54" s="8"/>
     </row>
     <row r="55" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A55" s="24"/>
+      <c r="A55" s="23"/>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
       <c r="E55" s="8"/>
     </row>
     <row r="56" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A56" s="24"/>
+      <c r="A56" s="23"/>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
       <c r="E56" s="8"/>
     </row>
     <row r="57" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A57" s="24"/>
+      <c r="A57" s="23"/>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
       <c r="E57" s="8"/>
     </row>
     <row r="58" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A58" s="24"/>
+      <c r="A58" s="23"/>
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
@@ -4829,21 +4885,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F99"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="3" width="14.5" style="3"/>
     <col min="4" max="4" width="15.6640625" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="14.5" style="3"/>
+    <col min="5" max="5" width="17.33203125" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="14.5" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>288</v>
       </c>
@@ -4851,141 +4908,197 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="22" t="s">
+        <v>289</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>333</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>334</v>
+      </c>
+      <c r="D2" s="4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="25" t="s">
+        <v>335</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>336</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>337</v>
+      </c>
+      <c r="D3" s="4">
+        <v>15</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>289</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>327</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="J3" s="13" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="23" t="s">
+    <row r="4" spans="1:10" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="25" t="s">
+        <v>338</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>339</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>340</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>341</v>
+      </c>
+      <c r="F4" s="22" t="s">
         <v>289</v>
       </c>
-      <c r="B2" s="27" t="s">
-        <v>297</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>306</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="26" t="s">
-        <v>292</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>298</v>
-      </c>
-      <c r="C3" s="18" t="s">
+      <c r="G4" s="26" t="s">
         <v>293</v>
       </c>
-      <c r="D3" s="18" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="17" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="26" t="s">
-        <v>296</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>304</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>303</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="23" t="s">
+      <c r="H4" s="17" t="s">
+        <v>327</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="22" t="s">
+        <v>342</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>343</v>
+      </c>
+      <c r="C5" s="17">
+        <v>2001</v>
+      </c>
+      <c r="D5" s="4">
+        <v>10</v>
+      </c>
+      <c r="F5" s="22" t="s">
         <v>289</v>
       </c>
-      <c r="B5" s="28" t="s">
-        <v>307</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>308</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="G5" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>327</v>
+      </c>
+      <c r="I5" s="4">
         <v>30</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="14"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="F6" s="3" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="14"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="J5" s="13" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="22" t="s">
+        <v>344</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>345</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>346</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>289</v>
+      </c>
+      <c r="G6" s="26" t="s">
+        <v>293</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>327</v>
+      </c>
+      <c r="I6" s="4">
+        <v>30</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="22"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="17"/>
       <c r="D7" s="4"/>
-      <c r="F7" s="3" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="14"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="14"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="14"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="14"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="14"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="14"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="14"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="14"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="14"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -5033,13 +5146,13 @@
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="14"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="14"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -5488,6 +5601,18 @@
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
+    </row>
+    <row r="100" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+      <c r="A100" s="14"/>
+      <c r="B100" s="4"/>
+      <c r="C100" s="4"/>
+      <c r="D100" s="4"/>
+    </row>
+    <row r="101" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+      <c r="A101" s="14"/>
+      <c r="B101" s="4"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5506,12 +5631,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="34"/>
-    <col min="9" max="16384" width="10.83203125" style="32"/>
+    <col min="1" max="1" width="10.83203125" style="32"/>
+    <col min="9" max="16384" width="10.83203125" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.15">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="31" t="s">
         <v>280</v>
       </c>
       <c r="B1" s="11">
@@ -5532,440 +5657,440 @@
       <c r="G1" s="11">
         <v>2016</v>
       </c>
-      <c r="H1" s="31">
+      <c r="H1" s="29">
         <v>2017</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="33" t="s">
         <v>287</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33" t="s">
         <v>287</v>
       </c>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="33" t="s">
         <v>287</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35" t="s">
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33" t="s">
         <v>287</v>
       </c>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35" t="s">
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33" t="s">
         <v>287</v>
       </c>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35" t="s">
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="33" t="s">
         <v>287</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="33" t="s">
         <v>287</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35" t="s">
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33" t="s">
         <v>287</v>
       </c>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="32" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="32" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="32" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="32" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="32" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="32" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="32" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="32" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="32" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="32" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="32" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="32" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="32" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="32" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="32" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="32" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="32" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="32" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A25" s="34" t="s">
+      <c r="A25" s="32" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="32" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="32" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A28" s="34" t="s">
+      <c r="A28" s="32" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="32" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A30" s="34" t="s">
+      <c r="A30" s="32" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="32" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="32" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A33" s="34" t="s">
+      <c r="A33" s="32" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A34" s="34" t="s">
+      <c r="A34" s="32" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="32" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="32" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A37" s="34" t="s">
+      <c r="A37" s="32" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A38" s="34" t="s">
+      <c r="A38" s="32" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A39" s="34" t="s">
+      <c r="A39" s="32" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A40" s="34" t="s">
+      <c r="A40" s="32" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A41" s="34" t="s">
+      <c r="A41" s="32" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="32" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="32" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A44" s="34" t="s">
+      <c r="A44" s="32" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A45" s="34" t="s">
+      <c r="A45" s="32" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A46" s="34" t="s">
+      <c r="A46" s="32" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A47" s="34" t="s">
+      <c r="A47" s="32" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A48" s="34" t="s">
+      <c r="A48" s="32" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A49" s="34" t="s">
+      <c r="A49" s="32" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A50" s="34" t="s">
+      <c r="A50" s="32" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A51" s="34" t="s">
+      <c r="A51" s="32" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A52" s="34" t="s">
+      <c r="A52" s="32" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A53" s="34" t="s">
+      <c r="A53" s="32" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A54" s="34" t="s">
+      <c r="A54" s="32" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A55" s="34" t="s">
+      <c r="A55" s="32" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A56" s="34" t="s">
+      <c r="A56" s="32" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A57" s="34" t="s">
+      <c r="A57" s="32" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A58" s="34" t="s">
+      <c r="A58" s="32" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A59" s="34" t="s">
+      <c r="A59" s="32" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A60" s="34" t="s">
+      <c r="A60" s="32" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A61" s="34" t="s">
+      <c r="A61" s="32" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A62" s="34" t="s">
+      <c r="A62" s="32" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A63" s="34" t="s">
+      <c r="A63" s="32" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A64" s="34" t="s">
+      <c r="A64" s="32" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A65" s="34" t="s">
+      <c r="A65" s="32" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A66" s="34" t="s">
+      <c r="A66" s="32" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A67" s="34" t="s">
+      <c r="A67" s="32" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A68" s="34" t="s">
+      <c r="A68" s="32" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A69" s="34" t="s">
+      <c r="A69" s="32" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A70" s="34" t="s">
+      <c r="A70" s="32" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A71" s="34" t="s">
+      <c r="A71" s="32" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A72" s="34" t="s">
+      <c r="A72" s="32" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A73" s="34" t="s">
+      <c r="A73" s="32" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A74" s="34" t="s">
+      <c r="A74" s="32" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A75" s="34" t="s">
+      <c r="A75" s="32" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A76" s="34" t="s">
+      <c r="A76" s="32" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A77" s="34" t="s">
+      <c r="A77" s="32" t="s">
         <v>104</v>
       </c>
     </row>
@@ -5992,78 +6117,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="17"/>
+      <c r="A2" s="16"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="19" t="s">
         <v>282</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="20" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="19" t="s">
         <v>283</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="21"/>
+      <c r="D5" s="20"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="19" t="s">
         <v>284</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="22"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="20"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="20"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
     </row>
     <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.15">
-      <c r="A14" s="22"/>
+      <c r="A14" s="21"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="20"/>
+      <c r="A15" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>